<commit_message>
removed bug: on grid view from user profile. click on post starts ActivityPost truly.
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -1314,10 +1314,10 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -1603,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105:XFD107"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1648,7 +1648,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
@@ -1659,7 +1659,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
@@ -1670,7 +1670,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
@@ -1689,7 +1689,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
@@ -1700,7 +1700,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="75">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1710,7 +1710,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45">
+    <row r="11" spans="1:4" ht="30">
       <c r="A11" s="18" t="s">
         <v>18</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="18" t="s">
         <v>24</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="60">
+    <row r="28" spans="1:4" ht="45">
       <c r="A28" s="18" t="s">
         <v>43</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45">
+    <row r="38" spans="1:4" ht="30">
       <c r="A38" s="4" t="s">
         <v>57</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45">
+    <row r="39" spans="1:4" ht="30">
       <c r="A39" s="18" t="s">
         <v>59</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="90">
+    <row r="41" spans="1:4" ht="75">
       <c r="A41" s="4" t="s">
         <v>63</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="76.5">
+    <row r="42" spans="1:4" ht="75.75">
       <c r="A42" s="4" t="s">
         <v>63</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="76.5">
+    <row r="43" spans="1:4" ht="75.75">
       <c r="A43" s="4" t="s">
         <v>70</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="76.5">
+    <row r="44" spans="1:4" ht="75.75">
       <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
@@ -2328,7 +2328,7 @@
       <c r="A78" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B78" s="23" t="s">
+      <c r="B78" s="24" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2336,19 +2336,19 @@
       <c r="A79" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="23"/>
+      <c r="B79" s="24"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="23"/>
+      <c r="B80" s="24"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="23"/>
+      <c r="B81" s="24"/>
     </row>
     <row r="82" spans="1:3" ht="300">
       <c r="A82" s="19" t="s">
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="105">
-      <c r="A104" s="24" t="s">
+      <c r="A104" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B104" t="s">
@@ -2517,9 +2517,8 @@
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="24"/>
+      <c r="A105" s="23"/>
       <c r="B105" s="9"/>
-      <c r="C105" s="8"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="5"/>

</xml_diff>

<commit_message>
webservices_bugs.xlsx : format changed!
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -12,9 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TODO" sheetId="2" r:id="rId1"/>
+    <sheet name="Trash" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="225">
   <si>
     <t>UnFollowBusiness</t>
   </si>
@@ -1153,12 +1155,645 @@
   <si>
     <t>type: bug</t>
   </si>
+  <si>
+    <t>5.31.2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comment on post by business</t>
+  </si>
+  <si>
+    <t>business.id: int
+post.id: int
+comment: String</t>
+  </si>
+  <si>
+    <t>report hint</t>
+  </si>
+  <si>
+    <t>report needs</t>
+  </si>
+  <si>
+    <t>extra Details</t>
+  </si>
+  <si>
+    <t>Action Status</t>
+  </si>
+  <si>
+    <t>report type</t>
+  </si>
+  <si>
+    <t>action Confirmation</t>
+  </si>
+  <si>
+    <t>search: "arayeshgah"</t>
+  </si>
+  <si>
+    <t>I updated a post with these data:
+{"Picture":"","Description":"dhhhdh@dhdhs.com\n","Price":"100,000"
+,"HashTagList":"hdhd","Discount":"0","PostId":"3146","Code":"dhdhhhddh"
+,"Title":"poooooost update"}
+after updating I ran the GetPost webservice</t>
+  </si>
+  <si>
+    <t>It returns the own user as friend</t>
+  </si>
+  <si>
+    <t>faulty data</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>bug</t>
+  </si>
+  <si>
+    <t>Confirmed!</t>
+  </si>
+  <si>
+    <t>redundant</t>
+  </si>
+  <si>
+    <t>Action Review Status</t>
+  </si>
+  <si>
+    <t>Reviewed!</t>
+  </si>
+  <si>
+    <t>NOT Confirmed!</t>
+  </si>
+  <si>
+    <t>Report Number</t>
+  </si>
+  <si>
+    <t>sample url:
+http://185.55.226.223:8081/bsn/deletePost/2/52
+{"Error":{"ErrorCode":"10"},"Result":"False","SuccessStatus":false}</t>
+  </si>
+  <si>
+    <r>
+      <t>sample URL:
+http://185.55.226.223:8081/bsn/getBusinessContactInfo/2
+returns website as null
+{"Phone":"www.google.com","Email":"sd@xxx.com","</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Website":null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,"Mobile":"11111111","Latitude":35.6975323181562,"WorkTimeClose":"17:00","Longitude":51.3911837339401,"WorkTimeOpen":"08:00"}</t>
+    </r>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getBlockedUsersList/2
+Endpoint not found.</t>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getBusinessContactInfo/1
+{"Error":{"ErrorCode":"08"},"Result":"","SuccessStatus":false}: it is a Get not Post</t>
+  </si>
+  <si>
+    <r>
+      <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserHomeInfo/2023/2019
+There is no record in db for user.id=2023 and user.id=2019 but the FriendshipRelationStatusCode is 4 that is wrong. It should be 2 (not friend)
+{"Error":{"ErrorCode":null},"Result":"{\"Name\":\"abkaveh\",\"AboutMe\":null,\"ProfilePictureId\
+":3189,\"CoverPictureId\":0,\"FriendRequestNumber\":0,\"FollowedBusinessNumber\":0,
+\"FriendsNumber\":0,\"ReviewsNumber\":0,\"Permission\":\"{\\\"Friends\\\":true,\\\"Reviews
+\\\":true,\\\"FollowedBusinesses\\\":true}\",\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>FriendshipRelationStatusCode\":4,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>\"Businesses\
+":null,\"UserId\":\"ab.kaveh\"}","SuccessStatus":true}</t>
+    </r>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getAllCommentNotifications/3/0/20
+It returns empty result
+{"Error":{"ErrorCode":null},"Result":"[]","SuccessStatus":true}</t>
+  </si>
+  <si>
+    <r>
+      <t>sample URL:
+http://185.55.226.223:8081/bsn/getBusinessReviews/3030/0/20
+wrong usreId:int. Users how reviewed the business are userId:2029 and userId:2030 not userId:1012 and userId:1014
+{"Error":{"ErrorCode":null},"Result":"[{\"Rate\":5,\"ReviewId\":1014,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\"UserId\":1014,\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"UserName\":\"hamid2\",\"UserProfilePictureId\":3247,\"Text\":\"بسیار هم عالیه\",\"Like\":0},{\"Rate\":5,\"ReviewId\":1012,\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"UserId\":1012,\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"UserName\":\"hamid1\",\"UserProfilePictureId\":0,\"Text\":\"خیلی خوبه\",\"Like\":0}]","SuccessStatus":true}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">sample URL:
+http://185.55.226.223:8081/bsn/getWallPosts/2030/0/20
+the user didn't share the following  posts but "IsLiked" is true for all of them
+….\"PostId\":1086…..
+…."PostId\":1085,…..
+…..\"PostId\":1084,….
+…..\"PostId\":1083,…..
+</t>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/commentOnPost/2019/1058/test
+The userId=2019 is blocked by the post's owner (businessId=2) but he can send comment on post</t>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/searchBusinessByLocation/hamidfastfood/11/35.84993291495611/51.66665095835924/0/20
+It doesn’t return  result while there is a business with businessId: "arayeshgah"</t>
+  </si>
+  <si>
+    <r>
+      <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendList/2029
+1. Returns the own user as his friend
+2. Returns some user's profilePictureId = 0
+{\"Id\":2036,\"UserId\":\"hamid5\",\"UserName\":\"hamid5\",\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserProfilePictureId\":0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,{\"Id\":2037,\"UserId\":\"hamid6\",\"UserName\":\"hamid6\",\"UserProfilePictureId\":0},{\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Id\":2029</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,\"UserId\":\"hamid1\",\"UserName\":\"hamid1\",\"UserProfilePictureId\":4313}</t>
+    </r>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/cancelShare/3/27
+{"Error":{"ErrorCode":"Value cannot be null.\u000d\u000aParameter name: entity"},"Result":"False","SuccessStatus":false}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">It returns UserId=1 while the userId=3
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">sample URL:
+http://185.55.226.223:8081/bsn/getWallPosts/3/0/20
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+It returns IsLiked = true for PostId=27 while it is false
+\"UserId\":1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+\"CommentNumber\":22,
+\"LikeNumber\":0,
+\"ShareNumber\":0,
+\"UserName\":\"sss\",
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\"PostId\":27,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+\"PostTypeId\":1,
+\"BusinessId\":1,
+\"BusinessUserName\":\"dkad\",
+\"CreationDate\":\"1821\",
+\"Title\":\"post3\",
+\"PostPictureId\":2022,
+\"BusinessProfilePictureId\":2022,
+\"Code\":\"5214\",
+\"Description\":\"des3\",
+\"Price\":\"123\",
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\"IsLiked\":true,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getWallPosts/2029/0/20
+returns 30 items instead of 20 (limitation)</t>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getWallPosts/2029/0/20
+returns some items twice like postId=1079  and postId=1068</t>
+  </si>
+  <si>
+    <r>
+      <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendRequestList/2029
+It returns all UserProfilePictureId = 2022
+[{\"Id\":2034,\"UserId\":\"hamid3\",\"UserName\":\"hamid3\",\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserProfilePictureId\":2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>},{\"Id\":2036,\"UserId\":\"hamid5\",\"UserName\":\"hamid5\",\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"UserProfilePictureId\":2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>},{\"Id\":2037,\"UserId\":\"hamid6\",\"UserName\":\"hamid6\",\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"UserProfilePictureId\":2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>},{\"Id\":4066,\"UserId\":\"tessst\",\"UserName\":\"تست\",\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserProfilePictureId\":2022}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,{\"Id\":3,\"UserId\":\"aliUserId\",\"UserName\":\"sss\",\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserProfilePictureId\":2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendList/2029
+It returns all UserProfilePictureId = 2022
+[{\"Id\":2034,\"UserId\":\"hamid3\",\"UserName\":\"hamid3\",\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserProfilePictureId\":2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>},{\"Id\":2036,\"UserId\":\"hamid5\",\"UserName\":\"hamid5\",\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserProfilePictureId\":2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>},{\"Id\":2037,\"UserId\":\"hamid6\",\"UserName\":\"hamid6\",\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserProfilePictureId\":2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendList/2034
+The result should be like this: Id=2029 &amp; UserId = "hamid1"
+[{\"Id\":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>2034</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>,\"UserId\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>":\"hamid3\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>",\"UserName\":\"hamid3\",\"UserProfilePictureId\":2022}]</t>
+    </r>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/deleteBusiness/5058/2029
+{"Error":{"ErrorCode":"10"},"Result":"False","SuccessStatus":false}</t>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserPost/2029/3146
+After update, GetPost returns the PostPictureId = 5512 which is NOT exist.
+It happens whenever I update a post.
+the result:
+{"Error":{"ErrorCode":null},"Result":"{\"UserId\":2029,\"BusinessId\":5059,\"PostId\":3146,\"UserName\":\"hamid1\",\"BusinessName\":null,\"Title\":\"poooooost update\",\"CreationDate\":\"0\",\"PostPictureId\":5512,\"BusinessProfilePictureId\":5508,\"Code\":\"dhdhhhddh\",\"Price\":\"100,000\",\"Comments\":\"[]\",\"Description\":\"dhhhdh@dhdhs.com\\n\",\"IsLiked\":false,\"IsShared\":false,\"IsReported\":false,\"HashTagList\":\"hdhd\"}","SuccessStatus":true}</t>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendList/2041
+"Result":"[{\"Id\":2041,\"UserId\":\"hamid10\",\"UserName\":\"hamid10\",\"UserProfilePictureId\":3258}
+,{\"Id\":2041,\"UserId\":\"hamid10\",\"UserName\":\"hamid10\",\"UserProfilePictureId\":3258}]</t>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getBusinessReviews/3030/0/20
+Endpoint  not found</t>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserHomeInfo/2036/2029 
+returns faulty data:
+{"Error":{"ErrorCode":"Sequence contains more than one element"},"Result":"","SuccessStatus":false}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1263,8 +1898,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1333,8 +1990,25 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1342,19 +2016,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="58">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1364,9 +2064,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1380,34 +2086,149 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="4" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="7">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="5">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="6">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="11">
+    <cellStyle name="20% - Accent1" xfId="10" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="9" builtinId="29"/>
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
-    <cellStyle name="Bad" xfId="6" builtinId="27"/>
-    <cellStyle name="Good" xfId="5" builtinId="26"/>
+    <cellStyle name="Bad" xfId="6" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="5" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="7" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Style 1" xfId="3"/>
     <cellStyle name="Style 2" xfId="4"/>
   </cellStyles>
@@ -1687,10 +2508,1920 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A2:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="39" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" style="39" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" s="32" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A2" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30.75" thickTop="1">
+      <c r="A3" s="31">
+        <v>1</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="31">
+        <v>2</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="31">
+        <v>3</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="31">
+        <v>4</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="31">
+        <v>5</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="31">
+        <v>6</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="31">
+        <v>7</v>
+      </c>
+      <c r="C9"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="31">
+        <v>8</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="31">
+        <v>9</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75">
+      <c r="A12" s="31">
+        <v>10</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="90">
+      <c r="A13" s="31">
+        <v>11</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="165">
+      <c r="A14" s="31">
+        <v>12</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="41"/>
+      <c r="G14" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H14" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="75">
+      <c r="A15" s="31">
+        <v>13</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H15" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="31">
+        <v>14</v>
+      </c>
+      <c r="C16"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="31">
+        <v>15</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+    </row>
+    <row r="18" spans="1:8" s="35" customFormat="1">
+      <c r="A18" s="35">
+        <v>16</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+    </row>
+    <row r="19" spans="1:8" ht="45">
+      <c r="A19" s="31">
+        <v>17</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" s="41"/>
+    </row>
+    <row r="20" spans="1:8" ht="45">
+      <c r="A20" s="31">
+        <v>18</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="41"/>
+    </row>
+    <row r="21" spans="1:8" ht="45">
+      <c r="A21" s="31">
+        <v>19</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="41"/>
+    </row>
+    <row r="22" spans="1:8" ht="105">
+      <c r="A22" s="31">
+        <v>20</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="F22" s="41"/>
+      <c r="G22" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="31">
+        <v>21</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="41"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="31">
+        <v>22</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24" s="49"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="31">
+        <v>23</v>
+      </c>
+      <c r="C25" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+    </row>
+    <row r="26" spans="1:8" ht="345">
+      <c r="A26" s="31">
+        <v>24</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" s="41"/>
+      <c r="G26" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H26" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60">
+      <c r="A27" s="31">
+        <v>25</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="G27" s="41"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="31">
+        <v>26</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G28" s="41"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="31">
+        <v>27</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" s="41"/>
+    </row>
+    <row r="30" spans="1:8" ht="60">
+      <c r="A30" s="31">
+        <v>28</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="41"/>
+      <c r="G30" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H30" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="47" customFormat="1" ht="105">
+      <c r="A31" s="47">
+        <v>29</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="57" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="31">
+        <v>30</v>
+      </c>
+      <c r="C32"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="31">
+        <v>31</v>
+      </c>
+      <c r="C33" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+    </row>
+    <row r="34" spans="1:8" ht="210">
+      <c r="A34" s="31">
+        <v>32</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="41"/>
+      <c r="G34" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30">
+      <c r="A35" s="31">
+        <v>33</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="41"/>
+    </row>
+    <row r="36" spans="1:8" ht="195">
+      <c r="A36" s="31">
+        <v>34</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="41"/>
+      <c r="G36" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H36" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="31">
+        <v>35</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G37" s="41"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="31">
+        <v>36</v>
+      </c>
+      <c r="C38"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="31">
+        <v>37</v>
+      </c>
+      <c r="C39" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+    </row>
+    <row r="40" spans="1:8" ht="45">
+      <c r="A40" s="31">
+        <v>38</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="G40" s="41"/>
+    </row>
+    <row r="41" spans="1:8" ht="45">
+      <c r="A41" s="31">
+        <v>39</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="41"/>
+      <c r="G41" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H41" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="45">
+      <c r="A42" s="31">
+        <v>40</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G42" s="41"/>
+    </row>
+    <row r="43" spans="1:8" ht="90">
+      <c r="A43" s="31">
+        <v>41</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="G43" s="41"/>
+    </row>
+    <row r="44" spans="1:8" ht="75">
+      <c r="A44" s="31">
+        <v>42</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="51"/>
+      <c r="F44" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G44" s="41"/>
+    </row>
+    <row r="45" spans="1:8" ht="75">
+      <c r="A45" s="31">
+        <v>43</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="51"/>
+      <c r="F45" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G45" s="41"/>
+    </row>
+    <row r="46" spans="1:8" ht="75">
+      <c r="A46" s="31">
+        <v>44</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="51"/>
+      <c r="F46" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G46" s="41"/>
+    </row>
+    <row r="47" spans="1:8" ht="285">
+      <c r="A47" s="31">
+        <v>45</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H47" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="180">
+      <c r="A48" s="31">
+        <v>46</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="F48" s="41"/>
+      <c r="G48" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H48" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="31">
+        <v>47</v>
+      </c>
+      <c r="C49"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="31">
+        <v>48</v>
+      </c>
+      <c r="C50" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
+    </row>
+    <row r="51" spans="1:8" ht="105">
+      <c r="A51" s="31">
+        <v>49</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="F51" s="41"/>
+      <c r="G51" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H51" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="31">
+        <v>50</v>
+      </c>
+      <c r="B52" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C52" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="41"/>
+      <c r="G52" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H52" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="31">
+        <v>51</v>
+      </c>
+      <c r="C53"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="31">
+        <v>52</v>
+      </c>
+      <c r="C54" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" s="41"/>
+      <c r="G54" s="41"/>
+    </row>
+    <row r="55" spans="1:8" ht="60">
+      <c r="A55" s="31">
+        <v>53</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F55" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G55" s="41"/>
+    </row>
+    <row r="56" spans="1:8" ht="30">
+      <c r="A56" s="31">
+        <v>54</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+    </row>
+    <row r="57" spans="1:8" ht="75">
+      <c r="A57" s="31">
+        <v>55</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C57" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F57" s="41"/>
+      <c r="G57" s="41"/>
+    </row>
+    <row r="58" spans="1:8" ht="90">
+      <c r="A58" s="31">
+        <v>56</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="F58" s="41"/>
+      <c r="G58" s="41"/>
+    </row>
+    <row r="59" spans="1:8" ht="30">
+      <c r="A59" s="31">
+        <v>57</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="F59" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="G59" s="41"/>
+    </row>
+    <row r="60" spans="1:8" ht="45">
+      <c r="A60" s="31">
+        <v>58</v>
+      </c>
+      <c r="B60" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F60" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" s="41"/>
+    </row>
+    <row r="61" spans="1:8" ht="30">
+      <c r="A61" s="31">
+        <v>59</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C61" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G61" s="41"/>
+    </row>
+    <row r="62" spans="1:8" ht="45">
+      <c r="A62" s="31">
+        <v>60</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C62" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F62" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G62" s="41"/>
+    </row>
+    <row r="63" spans="1:8" ht="45">
+      <c r="A63" s="31">
+        <v>61</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C63" t="s">
+        <v>96</v>
+      </c>
+      <c r="D63" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="G63" s="41"/>
+    </row>
+    <row r="64" spans="1:8" ht="45">
+      <c r="A64" s="31">
+        <v>62</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="F64" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G64" s="41"/>
+    </row>
+    <row r="65" spans="1:8" ht="135">
+      <c r="A65" s="31">
+        <v>63</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C65" t="s">
+        <v>93</v>
+      </c>
+      <c r="D65" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="E65" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="F65" s="41"/>
+      <c r="G65" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H65" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="60">
+      <c r="A66" s="31">
+        <v>64</v>
+      </c>
+      <c r="B66" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" t="s">
+        <v>100</v>
+      </c>
+      <c r="D66" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="E66" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="F66" s="41"/>
+      <c r="G66" s="41"/>
+    </row>
+    <row r="67" spans="1:8" ht="60">
+      <c r="A67" s="31">
+        <v>65</v>
+      </c>
+      <c r="B67" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" t="s">
+        <v>103</v>
+      </c>
+      <c r="D67" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E67" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="F67" s="41"/>
+      <c r="G67" s="41"/>
+    </row>
+    <row r="68" spans="1:8" ht="30">
+      <c r="A68" s="31">
+        <v>66</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" t="s">
+        <v>106</v>
+      </c>
+      <c r="D68" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E68" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="G68" s="41"/>
+    </row>
+    <row r="69" spans="1:8" ht="30">
+      <c r="A69" s="31">
+        <v>67</v>
+      </c>
+      <c r="B69" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C69" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="E69" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F69" s="41"/>
+      <c r="G69" s="41"/>
+    </row>
+    <row r="70" spans="1:8" ht="30">
+      <c r="A70" s="31">
+        <v>68</v>
+      </c>
+      <c r="B70" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C70" t="s">
+        <v>111</v>
+      </c>
+      <c r="D70" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="F70" s="41"/>
+      <c r="G70" s="41"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="31">
+        <v>69</v>
+      </c>
+      <c r="C71"/>
+      <c r="F71" s="41"/>
+      <c r="G71" s="41"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="31">
+        <v>70</v>
+      </c>
+      <c r="C72" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="F72" s="41"/>
+      <c r="G72" s="41"/>
+    </row>
+    <row r="73" spans="1:8" ht="240">
+      <c r="A73" s="31">
+        <v>71</v>
+      </c>
+      <c r="B73" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="F73" s="41"/>
+      <c r="G73" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H73" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="31">
+        <v>72</v>
+      </c>
+      <c r="B74" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C74" t="s">
+        <v>116</v>
+      </c>
+      <c r="D74" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F74" s="41"/>
+      <c r="G74" s="41"/>
+    </row>
+    <row r="75" spans="1:8" ht="30">
+      <c r="A75" s="31">
+        <v>73</v>
+      </c>
+      <c r="B75" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C75" t="s">
+        <v>106</v>
+      </c>
+      <c r="D75" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="F75" s="41"/>
+      <c r="G75" s="41"/>
+    </row>
+    <row r="76" spans="1:8" ht="120">
+      <c r="A76" s="31">
+        <v>74</v>
+      </c>
+      <c r="B76" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C76" t="s">
+        <v>120</v>
+      </c>
+      <c r="E76" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="F76" s="41"/>
+      <c r="G76" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H76" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="409.5">
+      <c r="A77" s="31">
+        <v>75</v>
+      </c>
+      <c r="B77" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C77" t="s">
+        <v>124</v>
+      </c>
+      <c r="E77" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="F77" s="41"/>
+      <c r="G77" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H77" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="90">
+      <c r="A78" s="31">
+        <v>76</v>
+      </c>
+      <c r="B78" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C78" t="s">
+        <v>124</v>
+      </c>
+      <c r="E78" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="F78" s="41"/>
+      <c r="G78" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H78" s="44" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="90">
+      <c r="A79" s="31">
+        <v>77</v>
+      </c>
+      <c r="B79" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C79" t="s">
+        <v>124</v>
+      </c>
+      <c r="E79" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="F79" s="41"/>
+      <c r="G79" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H79" s="44" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="31">
+        <v>78</v>
+      </c>
+      <c r="B80" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C80" t="s">
+        <v>30</v>
+      </c>
+      <c r="D80" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="F80" s="41"/>
+      <c r="G80" s="41"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="31">
+        <v>79</v>
+      </c>
+      <c r="B81" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C81" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" s="55"/>
+      <c r="F81" s="41"/>
+      <c r="G81" s="41"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="31">
+        <v>80</v>
+      </c>
+      <c r="B82" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D82" s="55"/>
+      <c r="F82" s="41"/>
+      <c r="G82" s="41"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="31">
+        <v>81</v>
+      </c>
+      <c r="B83" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" s="55"/>
+      <c r="F83" s="41"/>
+      <c r="G83" s="41"/>
+    </row>
+    <row r="84" spans="1:8" ht="300">
+      <c r="A84" s="31">
+        <v>82</v>
+      </c>
+      <c r="B84" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C84" t="s">
+        <v>129</v>
+      </c>
+      <c r="E84" s="45" t="s">
+        <v>217</v>
+      </c>
+      <c r="F84" s="41"/>
+      <c r="G84" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H84" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="225">
+      <c r="A85" s="31">
+        <v>83</v>
+      </c>
+      <c r="B85" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" t="s">
+        <v>131</v>
+      </c>
+      <c r="E85" s="45" t="s">
+        <v>218</v>
+      </c>
+      <c r="F85" s="41"/>
+      <c r="G85" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H85" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="31">
+        <v>84</v>
+      </c>
+      <c r="B86" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" t="s">
+        <v>59</v>
+      </c>
+      <c r="D86" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="E86" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="F86" s="41"/>
+      <c r="G86" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H86" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="31">
+        <v>85</v>
+      </c>
+      <c r="C87"/>
+      <c r="F87" s="41"/>
+      <c r="G87" s="41"/>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="31">
+        <v>86</v>
+      </c>
+      <c r="C88" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="F88" s="41"/>
+      <c r="G88" s="41"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="31">
+        <v>87</v>
+      </c>
+      <c r="B89" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C89" t="s">
+        <v>137</v>
+      </c>
+      <c r="D89" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F89" s="41"/>
+      <c r="G89" s="41"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="31">
+        <v>88</v>
+      </c>
+      <c r="C90"/>
+      <c r="F90" s="41"/>
+      <c r="G90" s="41"/>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="31">
+        <v>89</v>
+      </c>
+      <c r="C91" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="F91" s="41"/>
+      <c r="G91" s="41"/>
+    </row>
+    <row r="92" spans="1:8" ht="135">
+      <c r="A92" s="31">
+        <v>90</v>
+      </c>
+      <c r="B92" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C92" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="F92" s="41"/>
+      <c r="G92" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H92" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="60">
+      <c r="A93" s="31">
+        <v>91</v>
+      </c>
+      <c r="B93" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" t="s">
+        <v>137</v>
+      </c>
+      <c r="D93" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="F93" s="41"/>
+      <c r="G93" s="41"/>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="31">
+        <v>92</v>
+      </c>
+      <c r="C94"/>
+      <c r="F94" s="41"/>
+      <c r="G94" s="41"/>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="31">
+        <v>93</v>
+      </c>
+      <c r="C95" s="53" t="s">
+        <v>145</v>
+      </c>
+      <c r="F95" s="41"/>
+      <c r="G95" s="41"/>
+    </row>
+    <row r="96" spans="1:8" ht="90">
+      <c r="A96" s="31">
+        <v>94</v>
+      </c>
+      <c r="B96" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C96" t="s">
+        <v>146</v>
+      </c>
+      <c r="E96" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="F96" s="41"/>
+      <c r="G96" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="H96" s="43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="31">
+        <v>95</v>
+      </c>
+      <c r="C97"/>
+      <c r="D97" s="48"/>
+      <c r="E97" s="46"/>
+      <c r="F97" s="41"/>
+      <c r="G97" s="41"/>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="31">
+        <v>96</v>
+      </c>
+      <c r="C98" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="D98" s="48"/>
+      <c r="E98" s="46"/>
+      <c r="F98" s="41"/>
+      <c r="G98" s="41"/>
+    </row>
+    <row r="99" spans="1:7" ht="360">
+      <c r="A99" s="31">
+        <v>97</v>
+      </c>
+      <c r="B99" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C99" t="s">
+        <v>148</v>
+      </c>
+      <c r="D99" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="E99" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="F99" s="41"/>
+      <c r="G99" s="41"/>
+    </row>
+    <row r="100" spans="1:7" ht="150">
+      <c r="A100" s="31">
+        <v>98</v>
+      </c>
+      <c r="B100" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C100" t="s">
+        <v>151</v>
+      </c>
+      <c r="D100" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="E100" s="45" t="s">
+        <v>222</v>
+      </c>
+      <c r="F100" s="41"/>
+      <c r="G100" s="41"/>
+    </row>
+    <row r="101" spans="1:7" ht="255">
+      <c r="A101" s="31">
+        <v>99</v>
+      </c>
+      <c r="B101" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C101" t="s">
+        <v>154</v>
+      </c>
+      <c r="D101" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E101" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F101" s="41"/>
+      <c r="G101" s="41"/>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="31">
+        <v>100</v>
+      </c>
+      <c r="B102" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C102" t="s">
+        <v>156</v>
+      </c>
+      <c r="D102" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="F102" s="41"/>
+      <c r="G102" s="41"/>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="31">
+        <v>101</v>
+      </c>
+      <c r="C103"/>
+      <c r="F103" s="41"/>
+      <c r="G103" s="41"/>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="31">
+        <v>102</v>
+      </c>
+      <c r="C104" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="F104" s="41"/>
+      <c r="G104" s="41"/>
+    </row>
+    <row r="105" spans="1:7" ht="75">
+      <c r="A105" s="31">
+        <v>103</v>
+      </c>
+      <c r="B105" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C105" t="s">
+        <v>170</v>
+      </c>
+      <c r="E105" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="F105" s="41"/>
+      <c r="G105" s="41"/>
+    </row>
+    <row r="106" spans="1:7" ht="150">
+      <c r="A106" s="31">
+        <v>104</v>
+      </c>
+      <c r="B106" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="E106" s="45" t="s">
+        <v>224</v>
+      </c>
+      <c r="F106" s="41"/>
+      <c r="G106" s="41"/>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="31">
+        <v>105</v>
+      </c>
+      <c r="C107"/>
+      <c r="F107" s="41"/>
+      <c r="G107" s="41"/>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="31">
+        <v>106</v>
+      </c>
+      <c r="C108" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="F108" s="41"/>
+      <c r="G108" s="41"/>
+    </row>
+    <row r="109" spans="1:7" ht="45">
+      <c r="A109" s="31">
+        <v>107</v>
+      </c>
+      <c r="B109" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C109" t="s">
+        <v>182</v>
+      </c>
+      <c r="D109" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E109" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F109" s="41"/>
+      <c r="G109" s="41"/>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="31">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="31">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="31">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="31">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="31">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="31">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="31">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="31">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="31">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D80:D83"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E110"/>
+  <sheetViews>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1711,7 +4442,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1725,7 +4456,7 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1739,12 +4470,12 @@
       <c r="D3" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
@@ -1753,12 +4484,12 @@
       <c r="D4" t="s">
         <v>159</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
@@ -1767,12 +4498,12 @@
       <c r="D5" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
@@ -1784,7 +4515,7 @@
       <c r="D6" t="s">
         <v>160</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1794,7 +4525,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
@@ -1803,12 +4534,12 @@
       <c r="D9" t="s">
         <v>159</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="75">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1817,7 +4548,7 @@
       <c r="D10" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="26" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1831,7 +4562,7 @@
       <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="28" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1845,7 +4576,7 @@
       <c r="C12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="28" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1859,7 +4590,7 @@
       <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="28" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1893,7 +4624,7 @@
       <c r="D17" t="s">
         <v>161</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="26" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1907,7 +4638,7 @@
       <c r="D18" t="s">
         <v>162</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="26" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2115,7 +4846,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="75.75">
+    <row r="42" spans="1:4" ht="75">
       <c r="A42" s="4" t="s">
         <v>63</v>
       </c>
@@ -2127,7 +4858,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="75.75">
+    <row r="43" spans="1:4" ht="75">
       <c r="A43" s="4" t="s">
         <v>70</v>
       </c>
@@ -2139,7 +4870,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="75.75">
+    <row r="44" spans="1:4" ht="75">
       <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
@@ -2458,7 +5189,7 @@
       <c r="A78" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B78" s="25" t="s">
+      <c r="B78" s="54" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2466,19 +5197,19 @@
       <c r="A79" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="25"/>
+      <c r="B79" s="54"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="25"/>
+      <c r="B80" s="54"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="25"/>
+      <c r="B81" s="54"/>
     </row>
     <row r="82" spans="1:3" ht="300">
       <c r="A82" s="19" t="s">
@@ -2657,6 +5388,23 @@
     <row r="107" spans="1:3">
       <c r="A107" s="5"/>
       <c r="B107" s="9"/>
+    </row>
+    <row r="108" spans="1:3" ht="13.5" customHeight="1"/>
+    <row r="109" spans="1:3">
+      <c r="A109" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" s="30" customFormat="1" ht="45">
+      <c r="A110" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
some parametr names in PARAM.JAVA changed by refactor
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Trash" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="227">
   <si>
     <t>UnFollowBusiness</t>
   </si>
@@ -1176,13 +1175,7 @@
     <t>extra Details</t>
   </si>
   <si>
-    <t>Action Status</t>
-  </si>
-  <si>
     <t>report type</t>
-  </si>
-  <si>
-    <t>action Confirmation</t>
   </si>
   <si>
     <t>search: "arayeshgah"</t>
@@ -1211,9 +1204,6 @@
   </si>
   <si>
     <t>redundant</t>
-  </si>
-  <si>
-    <t>Action Review Status</t>
   </si>
   <si>
     <t>Reviewed!</t>
@@ -1787,6 +1777,26 @@
 http://185.55.226.223:8081/bsn/getUserHomeInfo/2036/2029 
 returns faulty data:
 {"Error":{"ErrorCode":"Sequence contains more than one element"},"Result":"","SuccessStatus":false}</t>
+  </si>
+  <si>
+    <t>Action
+Review
+Status</t>
+  </si>
+  <si>
+    <t>Action
+Confirmation</t>
+  </si>
+  <si>
+    <t>waiting for change!</t>
+  </si>
+  <si>
+    <t>Action
+Reported
+Status</t>
+  </si>
+  <si>
+    <t>{"LocationLongitude":"51.3911837339401","Phone":"555555555","Description":"ddddddddddd","HashTagList":"","CoverPicture":"","WorkTimeClose":"17:00","WorkDays":"1,5,6,7","ProfilePicture":"2022","City":"تهران","Name":"lk2222","Category":"cloth","Email":"sd@xxx.com","State":"تهران","Address":"آدرس","SubCategory":"men cloth","Mobile":"11111111","LocationLatitude":"35.6975323181562","WorkTimeOpen":"08:00"}</t>
   </si>
 </sst>
 </file>
@@ -2046,12 +2056,14 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2143,85 +2155,94 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="8" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="9" builtinId="29"/>
+    <cellStyle name="Accent1" xfId="9" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Bad" xfId="6" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Good" xfId="5" builtinId="26" customBuiltin="1"/>
@@ -2511,1899 +2532,1751 @@
   <dimension ref="A2:H118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="39" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" style="39" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" style="39" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="39" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="46" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="46" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" style="46" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="46" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="46" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="46" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="32" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A2" s="56" t="s">
+    <row r="2" spans="1:8" s="32" customFormat="1" ht="52.5" thickBot="1">
+      <c r="A2" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30.75" thickTop="1">
+      <c r="A3" s="52">
+        <v>1</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="52">
+        <v>2</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="52">
+        <v>3</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="52">
+        <v>4</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="52">
+        <v>5</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="52">
+        <v>6</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="52">
+        <v>8</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="52">
+        <v>9</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75">
+      <c r="A12" s="52">
+        <v>10</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H12" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="75">
+      <c r="A13" s="52">
+        <v>11</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>199</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="135">
+      <c r="A14" s="52">
+        <v>12</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="75">
+      <c r="A15" s="52">
+        <v>13</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="G15" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="52">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="52">
+        <v>15</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="33" customFormat="1">
+      <c r="A18" s="51">
+        <v>16</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+    </row>
+    <row r="19" spans="1:8" ht="45">
+      <c r="A19" s="52">
+        <v>17</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="H19" s="58" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45">
+      <c r="A20" s="52">
+        <v>18</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45">
+      <c r="A21" s="52">
+        <v>19</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="90">
+      <c r="A22" s="52">
+        <v>20</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H22" s="59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="52">
+        <v>21</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="52">
+        <v>22</v>
+      </c>
+      <c r="D24" s="42"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="52">
+        <v>23</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="42"/>
+    </row>
+    <row r="26" spans="1:8" ht="255">
+      <c r="A26" s="52">
+        <v>24</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H26" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60">
+      <c r="A27" s="52">
+        <v>25</v>
+      </c>
+      <c r="B27" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="46" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="52">
+        <v>26</v>
+      </c>
+      <c r="B28" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="52">
+        <v>27</v>
+      </c>
+      <c r="B29" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="60">
+      <c r="A30" s="52">
+        <v>28</v>
+      </c>
+      <c r="B30" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H30" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="40" customFormat="1" ht="105">
+      <c r="A31" s="51">
+        <v>29</v>
+      </c>
+      <c r="B31" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="56"/>
+      <c r="E31" s="60" t="s">
+        <v>204</v>
+      </c>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="52">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="52">
+        <v>31</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="165">
+      <c r="A34" s="52">
+        <v>32</v>
+      </c>
+      <c r="B34" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C34" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H34" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30">
+      <c r="A35" s="52">
+        <v>33</v>
+      </c>
+      <c r="B35" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="46" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="135">
+      <c r="A36" s="52">
+        <v>34</v>
+      </c>
+      <c r="B36" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="G36" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H36" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="52">
+        <v>35</v>
+      </c>
+      <c r="B37" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="52">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="52">
+        <v>37</v>
+      </c>
+      <c r="C39" s="45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="45">
+      <c r="A40" s="52">
+        <v>38</v>
+      </c>
+      <c r="B40" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="46" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="45">
+      <c r="A41" s="52">
+        <v>39</v>
+      </c>
+      <c r="B41" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="G41" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H41" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="45">
+      <c r="A42" s="52">
+        <v>40</v>
+      </c>
+      <c r="B42" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="90">
+      <c r="A43" s="52">
+        <v>41</v>
+      </c>
+      <c r="B43" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="46" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="75">
+      <c r="A44" s="52">
+        <v>42</v>
+      </c>
+      <c r="B44" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="44"/>
+      <c r="F44" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="75">
+      <c r="A45" s="52">
+        <v>43</v>
+      </c>
+      <c r="B45" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="44"/>
+      <c r="F45" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="75">
+      <c r="A46" s="52">
+        <v>44</v>
+      </c>
+      <c r="B46" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="44"/>
+      <c r="F46" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="225">
+      <c r="A47" s="52">
+        <v>45</v>
+      </c>
+      <c r="B47" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C47" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="G47" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="165">
+      <c r="A48" s="52">
+        <v>46</v>
+      </c>
+      <c r="B48" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C48" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="G48" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H48" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="52">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="52">
+        <v>48</v>
+      </c>
+      <c r="C50" s="45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="90">
+      <c r="A51" s="52">
+        <v>49</v>
+      </c>
+      <c r="B51" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="G51" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H51" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="52">
+        <v>50</v>
+      </c>
+      <c r="B52" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C52" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="G52" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H52" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="52">
+        <v>52</v>
+      </c>
+      <c r="C54" s="45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="60">
+      <c r="A55" s="52">
+        <v>53</v>
+      </c>
+      <c r="B55" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="F55" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="30">
+      <c r="A56" s="52">
+        <v>54</v>
+      </c>
+      <c r="B56" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" s="46" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="75">
+      <c r="A57" s="52">
+        <v>55</v>
+      </c>
+      <c r="B57" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C57" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="90">
+      <c r="A58" s="52">
+        <v>56</v>
+      </c>
+      <c r="B58" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C58" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="30">
+      <c r="A59" s="52">
+        <v>57</v>
+      </c>
+      <c r="B59" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="F59" s="46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="45">
+      <c r="A60" s="52">
+        <v>58</v>
+      </c>
+      <c r="B60" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="F60" s="46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="30">
+      <c r="A61" s="52">
+        <v>59</v>
+      </c>
+      <c r="B61" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C61" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="45">
+      <c r="A62" s="52">
+        <v>60</v>
+      </c>
+      <c r="B62" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C62" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="F62" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="45">
+      <c r="A63" s="52">
+        <v>61</v>
+      </c>
+      <c r="B63" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C63" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="D63" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63" s="46" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="45">
+      <c r="A64" s="52">
+        <v>62</v>
+      </c>
+      <c r="B64" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C64" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="F64" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="105">
+      <c r="A65" s="52">
+        <v>63</v>
+      </c>
+      <c r="B65" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D65" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="H2" s="37" t="s">
+      <c r="E65" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="G65" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H65" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="60">
+      <c r="A66" s="52">
+        <v>64</v>
+      </c>
+      <c r="B66" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="E66" s="46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="60">
+      <c r="A67" s="52">
+        <v>65</v>
+      </c>
+      <c r="B67" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="C67" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D67" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E67" s="46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="30">
+      <c r="A68" s="52">
+        <v>66</v>
+      </c>
+      <c r="B68" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="D68" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="E68" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="30">
+      <c r="A69" s="52">
+        <v>67</v>
+      </c>
+      <c r="B69" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C69" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E69" s="46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="30">
+      <c r="A70" s="52">
+        <v>68</v>
+      </c>
+      <c r="B70" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C70" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="D70" s="38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="52">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="52">
+        <v>70</v>
+      </c>
+      <c r="C72" s="45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="195">
+      <c r="A73" s="52">
+        <v>71</v>
+      </c>
+      <c r="B73" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="G73" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H73" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="52">
+        <v>72</v>
+      </c>
+      <c r="B74" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C74" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="D74" s="46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="30">
+      <c r="A75" s="52">
+        <v>73</v>
+      </c>
+      <c r="B75" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C75" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="D75" s="38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="90">
+      <c r="A76" s="52">
+        <v>74</v>
+      </c>
+      <c r="B76" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C76" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="E76" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="G76" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H76" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="390">
+      <c r="A77" s="52">
+        <v>75</v>
+      </c>
+      <c r="B77" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C77" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="E77" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="G77" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H77" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="75">
+      <c r="A78" s="52">
+        <v>76</v>
+      </c>
+      <c r="B78" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C78" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="E78" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="G78" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H78" s="59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="90">
+      <c r="A79" s="52">
+        <v>77</v>
+      </c>
+      <c r="B79" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C79" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="E79" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="G79" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H79" s="59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="52">
+        <v>78</v>
+      </c>
+      <c r="B80" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C80" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D80" s="48" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="52">
+        <v>79</v>
+      </c>
+      <c r="B81" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C81" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" s="48"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="52">
+        <v>80</v>
+      </c>
+      <c r="B82" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C82" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="D82" s="48"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="52">
+        <v>81</v>
+      </c>
+      <c r="B83" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" s="48"/>
+    </row>
+    <row r="84" spans="1:8" ht="225">
+      <c r="A84" s="52">
+        <v>82</v>
+      </c>
+      <c r="B84" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="E84" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="G84" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H84" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="180">
+      <c r="A85" s="52">
+        <v>83</v>
+      </c>
+      <c r="B85" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="E85" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="G85" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H85" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="52">
+        <v>84</v>
+      </c>
+      <c r="B86" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C86" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D86" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="E86" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="G86" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H86" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="52">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="52">
+        <v>86</v>
+      </c>
+      <c r="C88" s="45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="52">
+        <v>87</v>
+      </c>
+      <c r="B89" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C89" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="D89" s="46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="52">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="52">
+        <v>89</v>
+      </c>
+      <c r="C91" s="45" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="105">
+      <c r="A92" s="52">
+        <v>90</v>
+      </c>
+      <c r="B92" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C92" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="43" t="s">
+        <v>216</v>
+      </c>
+      <c r="G92" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H92" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="60">
+      <c r="A93" s="52">
+        <v>91</v>
+      </c>
+      <c r="B93" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="D93" s="38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="52">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="52">
+        <v>93</v>
+      </c>
+      <c r="C95" s="45" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="90">
+      <c r="A96" s="52">
+        <v>94</v>
+      </c>
+      <c r="B96" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C96" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="E96" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="G96" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="H96" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="52">
+        <v>95</v>
+      </c>
+      <c r="D97" s="41"/>
+      <c r="E97" s="39"/>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="52">
+        <v>96</v>
+      </c>
+      <c r="C98" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="D98" s="41"/>
+      <c r="E98" s="39"/>
+    </row>
+    <row r="99" spans="1:5" ht="285">
+      <c r="A99" s="52">
+        <v>97</v>
+      </c>
+      <c r="B99" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C99" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="D99" s="38" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="30.75" thickTop="1">
-      <c r="A3" s="31">
-        <v>1</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="40" t="s">
+      <c r="E99" s="38" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="120">
+      <c r="A100" s="52">
+        <v>98</v>
+      </c>
+      <c r="B100" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="D100" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="E100" s="38" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="255">
+      <c r="A101" s="52">
+        <v>99</v>
+      </c>
+      <c r="B101" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C101" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="D101" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E101" s="46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="52">
+        <v>100</v>
+      </c>
+      <c r="B102" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C102" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="D102" s="46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="52">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="52">
+        <v>102</v>
+      </c>
+      <c r="C104" s="45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="75">
+      <c r="A105" s="52">
+        <v>103</v>
+      </c>
+      <c r="B105" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C105" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="E105" s="38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="120">
+      <c r="A106" s="52">
+        <v>104</v>
+      </c>
+      <c r="B106" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C106" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="E106" s="38" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="52">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="52">
+        <v>106</v>
+      </c>
+      <c r="C108" s="45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="45">
+      <c r="A109" s="52">
+        <v>107</v>
+      </c>
+      <c r="B109" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="C109" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="D109" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="E109" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30">
-      <c r="A4" s="31">
-        <v>2</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="31">
-        <v>3</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G5" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="31">
-        <v>4</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="31">
-        <v>5</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G7" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H7" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="31">
-        <v>6</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="F8" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="G8" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="31">
-        <v>7</v>
-      </c>
-      <c r="C9"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="31">
-        <v>8</v>
-      </c>
-      <c r="C10" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="31">
-        <v>9</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="75">
-      <c r="A12" s="31">
-        <v>10</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G12" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H12" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="90">
-      <c r="A13" s="31">
-        <v>11</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="50" t="s">
-        <v>202</v>
-      </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H13" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="165">
-      <c r="A14" s="31">
-        <v>12</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>203</v>
-      </c>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H14" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="75">
-      <c r="A15" s="31">
-        <v>13</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H15" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="31">
-        <v>14</v>
-      </c>
-      <c r="C16"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="31">
-        <v>15</v>
-      </c>
-      <c r="C17" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-    </row>
-    <row r="18" spans="1:8" s="35" customFormat="1">
-      <c r="A18" s="35">
-        <v>16</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="C18" t="s">
-        <v>174</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-    </row>
-    <row r="19" spans="1:8" ht="45">
-      <c r="A19" s="31">
-        <v>17</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="52" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="41" t="s">
-        <v>161</v>
-      </c>
-      <c r="G19" s="41"/>
-    </row>
-    <row r="20" spans="1:8" ht="45">
-      <c r="A20" s="31">
-        <v>18</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="F20" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="G20" s="41"/>
-    </row>
-    <row r="21" spans="1:8" ht="45">
-      <c r="A21" s="31">
-        <v>19</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="G21" s="41"/>
-    </row>
-    <row r="22" spans="1:8" ht="105">
-      <c r="A22" s="31">
-        <v>20</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="50" t="s">
-        <v>205</v>
-      </c>
-      <c r="F22" s="41"/>
-      <c r="G22" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H22" s="44" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="31">
-        <v>21</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="G23" s="41"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="31">
-        <v>22</v>
-      </c>
-      <c r="C24"/>
-      <c r="D24" s="49"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="31">
-        <v>23</v>
-      </c>
-      <c r="C25" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="49"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-    </row>
-    <row r="26" spans="1:8" ht="345">
-      <c r="A26" s="31">
-        <v>24</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="50" t="s">
-        <v>206</v>
-      </c>
-      <c r="F26" s="41"/>
-      <c r="G26" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H26" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="60">
-      <c r="A27" s="31">
-        <v>25</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="G27" s="41"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="31">
-        <v>26</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G28" s="41"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="31">
-        <v>27</v>
-      </c>
-      <c r="B29" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G29" s="41"/>
-    </row>
-    <row r="30" spans="1:8" ht="60">
-      <c r="A30" s="31">
-        <v>28</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H30" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="47" customFormat="1" ht="105">
-      <c r="A31" s="47">
-        <v>29</v>
-      </c>
-      <c r="B31" s="47" t="s">
-        <v>197</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="57" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="31">
-        <v>30</v>
-      </c>
-      <c r="C32"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="31">
-        <v>31</v>
-      </c>
-      <c r="C33" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-    </row>
-    <row r="34" spans="1:8" ht="210">
-      <c r="A34" s="31">
-        <v>32</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="41"/>
-      <c r="G34" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H34" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="30">
-      <c r="A35" s="31">
-        <v>33</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="41" t="s">
-        <v>164</v>
-      </c>
-      <c r="G35" s="41"/>
-    </row>
-    <row r="36" spans="1:8" ht="195">
-      <c r="A36" s="31">
-        <v>34</v>
-      </c>
-      <c r="B36" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="41"/>
-      <c r="G36" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H36" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="31">
-        <v>35</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G37" s="41"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="31">
-        <v>36</v>
-      </c>
-      <c r="C38"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="31">
-        <v>37</v>
-      </c>
-      <c r="C39" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-    </row>
-    <row r="40" spans="1:8" ht="45">
-      <c r="A40" s="31">
-        <v>38</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C40" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="F40" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="G40" s="41"/>
-    </row>
-    <row r="41" spans="1:8" ht="45">
-      <c r="A41" s="31">
-        <v>39</v>
-      </c>
-      <c r="B41" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C41" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="F41" s="41"/>
-      <c r="G41" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H41" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="45">
-      <c r="A42" s="31">
-        <v>40</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C42" t="s">
-        <v>61</v>
-      </c>
-      <c r="D42" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="F42" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G42" s="41"/>
-    </row>
-    <row r="43" spans="1:8" ht="90">
-      <c r="A43" s="31">
-        <v>41</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C43" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="F43" s="41" t="s">
-        <v>166</v>
-      </c>
-      <c r="G43" s="41"/>
-    </row>
-    <row r="44" spans="1:8" ht="75">
-      <c r="A44" s="31">
-        <v>42</v>
-      </c>
-      <c r="B44" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C44" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E44" s="51"/>
-      <c r="F44" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G44" s="41"/>
-    </row>
-    <row r="45" spans="1:8" ht="75">
-      <c r="A45" s="31">
-        <v>43</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C45" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" s="51"/>
-      <c r="F45" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G45" s="41"/>
-    </row>
-    <row r="46" spans="1:8" ht="75">
-      <c r="A46" s="31">
-        <v>44</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C46" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E46" s="51"/>
-      <c r="F46" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G46" s="41"/>
-    </row>
-    <row r="47" spans="1:8" ht="285">
-      <c r="A47" s="31">
-        <v>45</v>
-      </c>
-      <c r="B47" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C47" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="F47" s="41"/>
-      <c r="G47" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H47" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="180">
-      <c r="A48" s="31">
-        <v>46</v>
-      </c>
-      <c r="B48" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C48" t="s">
-        <v>63</v>
-      </c>
-      <c r="E48" s="45" t="s">
-        <v>209</v>
-      </c>
-      <c r="F48" s="41"/>
-      <c r="G48" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H48" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="31">
-        <v>47</v>
-      </c>
-      <c r="C49"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="41"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="31">
-        <v>48</v>
-      </c>
-      <c r="C50" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41"/>
-    </row>
-    <row r="51" spans="1:8" ht="105">
-      <c r="A51" s="31">
-        <v>49</v>
-      </c>
-      <c r="B51" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C51" t="s">
-        <v>75</v>
-      </c>
-      <c r="E51" s="45" t="s">
-        <v>210</v>
-      </c>
-      <c r="F51" s="41"/>
-      <c r="G51" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H51" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="31">
-        <v>50</v>
-      </c>
-      <c r="B52" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C52" t="s">
-        <v>77</v>
-      </c>
-      <c r="D52" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="F52" s="41"/>
-      <c r="G52" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H52" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="31">
-        <v>51</v>
-      </c>
-      <c r="C53"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="31">
-        <v>52</v>
-      </c>
-      <c r="C54" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
-    </row>
-    <row r="55" spans="1:8" ht="60">
-      <c r="A55" s="31">
-        <v>53</v>
-      </c>
-      <c r="B55" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C55" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="E55" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="F55" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G55" s="41"/>
-    </row>
-    <row r="56" spans="1:8" ht="30">
-      <c r="A56" s="31">
-        <v>54</v>
-      </c>
-      <c r="B56" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C56" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="E56" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
-    </row>
-    <row r="57" spans="1:8" ht="75">
-      <c r="A57" s="31">
-        <v>55</v>
-      </c>
-      <c r="B57" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C57" t="s">
-        <v>85</v>
-      </c>
-      <c r="D57" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E57" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="F57" s="41"/>
-      <c r="G57" s="41"/>
-    </row>
-    <row r="58" spans="1:8" ht="90">
-      <c r="A58" s="31">
-        <v>56</v>
-      </c>
-      <c r="B58" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C58" t="s">
-        <v>21</v>
-      </c>
-      <c r="D58" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="F58" s="41"/>
-      <c r="G58" s="41"/>
-    </row>
-    <row r="59" spans="1:8" ht="30">
-      <c r="A59" s="31">
-        <v>57</v>
-      </c>
-      <c r="B59" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C59" t="s">
-        <v>89</v>
-      </c>
-      <c r="D59" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="F59" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="G59" s="41"/>
-    </row>
-    <row r="60" spans="1:8" ht="45">
-      <c r="A60" s="31">
-        <v>58</v>
-      </c>
-      <c r="B60" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C60" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="F60" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="G60" s="41"/>
-    </row>
-    <row r="61" spans="1:8" ht="30">
-      <c r="A61" s="31">
-        <v>59</v>
-      </c>
-      <c r="B61" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C61" t="s">
-        <v>92</v>
-      </c>
-      <c r="D61" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="F61" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G61" s="41"/>
-    </row>
-    <row r="62" spans="1:8" ht="45">
-      <c r="A62" s="31">
-        <v>60</v>
-      </c>
-      <c r="B62" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C62" t="s">
-        <v>93</v>
-      </c>
-      <c r="D62" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="F62" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G62" s="41"/>
-    </row>
-    <row r="63" spans="1:8" ht="45">
-      <c r="A63" s="31">
-        <v>61</v>
-      </c>
-      <c r="B63" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C63" t="s">
-        <v>96</v>
-      </c>
-      <c r="D63" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="F63" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="G63" s="41"/>
-    </row>
-    <row r="64" spans="1:8" ht="45">
-      <c r="A64" s="31">
-        <v>62</v>
-      </c>
-      <c r="B64" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="F64" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G64" s="41"/>
-    </row>
-    <row r="65" spans="1:8" ht="135">
-      <c r="A65" s="31">
-        <v>63</v>
-      </c>
-      <c r="B65" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C65" t="s">
-        <v>93</v>
-      </c>
-      <c r="D65" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="E65" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="F65" s="41"/>
-      <c r="G65" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H65" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="60">
-      <c r="A66" s="31">
-        <v>64</v>
-      </c>
-      <c r="B66" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="C66" t="s">
-        <v>100</v>
-      </c>
-      <c r="D66" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="E66" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="F66" s="41"/>
-      <c r="G66" s="41"/>
-    </row>
-    <row r="67" spans="1:8" ht="60">
-      <c r="A67" s="31">
-        <v>65</v>
-      </c>
-      <c r="B67" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="C67" t="s">
-        <v>103</v>
-      </c>
-      <c r="D67" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="E67" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="F67" s="41"/>
-      <c r="G67" s="41"/>
-    </row>
-    <row r="68" spans="1:8" ht="30">
-      <c r="A68" s="31">
-        <v>66</v>
-      </c>
-      <c r="B68" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C68" t="s">
-        <v>106</v>
-      </c>
-      <c r="D68" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="E68" s="39" t="s">
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="52">
         <v>108</v>
       </c>
-      <c r="F68" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G68" s="41"/>
-    </row>
-    <row r="69" spans="1:8" ht="30">
-      <c r="A69" s="31">
-        <v>67</v>
-      </c>
-      <c r="B69" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C69" t="s">
-        <v>64</v>
-      </c>
-      <c r="D69" s="45" t="s">
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="52">
         <v>109</v>
       </c>
-      <c r="E69" s="39" t="s">
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="52">
         <v>110</v>
       </c>
-      <c r="F69" s="41"/>
-      <c r="G69" s="41"/>
-    </row>
-    <row r="70" spans="1:8" ht="30">
-      <c r="A70" s="31">
-        <v>68</v>
-      </c>
-      <c r="B70" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C70" t="s">
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="52">
         <v>111</v>
       </c>
-      <c r="D70" s="45" t="s">
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="52">
         <v>112</v>
       </c>
-      <c r="F70" s="41"/>
-      <c r="G70" s="41"/>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="31">
-        <v>69</v>
-      </c>
-      <c r="C71"/>
-      <c r="F71" s="41"/>
-      <c r="G71" s="41"/>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="31">
-        <v>70</v>
-      </c>
-      <c r="C72" s="53" t="s">
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="52">
         <v>113</v>
       </c>
-      <c r="F72" s="41"/>
-      <c r="G72" s="41"/>
-    </row>
-    <row r="73" spans="1:8" ht="240">
-      <c r="A73" s="31">
-        <v>71</v>
-      </c>
-      <c r="B73" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C73" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="45" t="s">
-        <v>212</v>
-      </c>
-      <c r="F73" s="41"/>
-      <c r="G73" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H73" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="31">
-        <v>72</v>
-      </c>
-      <c r="B74" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C74" t="s">
-        <v>116</v>
-      </c>
-      <c r="D74" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="F74" s="41"/>
-      <c r="G74" s="41"/>
-    </row>
-    <row r="75" spans="1:8" ht="30">
-      <c r="A75" s="31">
-        <v>73</v>
-      </c>
-      <c r="B75" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C75" t="s">
-        <v>106</v>
-      </c>
-      <c r="D75" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="F75" s="41"/>
-      <c r="G75" s="41"/>
-    </row>
-    <row r="76" spans="1:8" ht="120">
-      <c r="A76" s="31">
-        <v>74</v>
-      </c>
-      <c r="B76" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C76" t="s">
-        <v>120</v>
-      </c>
-      <c r="E76" s="50" t="s">
-        <v>213</v>
-      </c>
-      <c r="F76" s="41"/>
-      <c r="G76" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H76" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="409.5">
-      <c r="A77" s="31">
-        <v>75</v>
-      </c>
-      <c r="B77" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C77" t="s">
-        <v>124</v>
-      </c>
-      <c r="E77" s="45" t="s">
-        <v>214</v>
-      </c>
-      <c r="F77" s="41"/>
-      <c r="G77" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H77" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="90">
-      <c r="A78" s="31">
-        <v>76</v>
-      </c>
-      <c r="B78" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C78" t="s">
-        <v>124</v>
-      </c>
-      <c r="E78" s="45" t="s">
-        <v>215</v>
-      </c>
-      <c r="F78" s="41"/>
-      <c r="G78" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H78" s="44" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="90">
-      <c r="A79" s="31">
-        <v>77</v>
-      </c>
-      <c r="B79" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C79" t="s">
-        <v>124</v>
-      </c>
-      <c r="E79" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H79" s="44" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="31">
-        <v>78</v>
-      </c>
-      <c r="B80" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C80" t="s">
-        <v>30</v>
-      </c>
-      <c r="D80" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="F80" s="41"/>
-      <c r="G80" s="41"/>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="31">
-        <v>79</v>
-      </c>
-      <c r="B81" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C81" t="s">
-        <v>29</v>
-      </c>
-      <c r="D81" s="55"/>
-      <c r="F81" s="41"/>
-      <c r="G81" s="41"/>
-    </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="31">
-        <v>80</v>
-      </c>
-      <c r="B82" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C82" t="s">
-        <v>63</v>
-      </c>
-      <c r="D82" s="55"/>
-      <c r="F82" s="41"/>
-      <c r="G82" s="41"/>
-    </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="31">
-        <v>81</v>
-      </c>
-      <c r="B83" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C83" t="s">
-        <v>16</v>
-      </c>
-      <c r="D83" s="55"/>
-      <c r="F83" s="41"/>
-      <c r="G83" s="41"/>
-    </row>
-    <row r="84" spans="1:8" ht="300">
-      <c r="A84" s="31">
-        <v>82</v>
-      </c>
-      <c r="B84" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C84" t="s">
-        <v>129</v>
-      </c>
-      <c r="E84" s="45" t="s">
-        <v>217</v>
-      </c>
-      <c r="F84" s="41"/>
-      <c r="G84" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H84" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="225">
-      <c r="A85" s="31">
-        <v>83</v>
-      </c>
-      <c r="B85" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C85" t="s">
-        <v>131</v>
-      </c>
-      <c r="E85" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="F85" s="41"/>
-      <c r="G85" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H85" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="31">
-        <v>84</v>
-      </c>
-      <c r="B86" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C86" t="s">
-        <v>59</v>
-      </c>
-      <c r="D86" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="E86" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="F86" s="41"/>
-      <c r="G86" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H86" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="31">
-        <v>85</v>
-      </c>
-      <c r="C87"/>
-      <c r="F87" s="41"/>
-      <c r="G87" s="41"/>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="31">
-        <v>86</v>
-      </c>
-      <c r="C88" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="F88" s="41"/>
-      <c r="G88" s="41"/>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="31">
-        <v>87</v>
-      </c>
-      <c r="B89" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C89" t="s">
-        <v>137</v>
-      </c>
-      <c r="D89" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="F89" s="41"/>
-      <c r="G89" s="41"/>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="31">
-        <v>88</v>
-      </c>
-      <c r="C90"/>
-      <c r="F90" s="41"/>
-      <c r="G90" s="41"/>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="31">
-        <v>89</v>
-      </c>
-      <c r="C91" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="F91" s="41"/>
-      <c r="G91" s="41"/>
-    </row>
-    <row r="92" spans="1:8" ht="135">
-      <c r="A92" s="31">
-        <v>90</v>
-      </c>
-      <c r="B92" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C92" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="F92" s="41"/>
-      <c r="G92" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H92" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="60">
-      <c r="A93" s="31">
-        <v>91</v>
-      </c>
-      <c r="B93" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C93" t="s">
-        <v>137</v>
-      </c>
-      <c r="D93" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="F93" s="41"/>
-      <c r="G93" s="41"/>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="A94" s="31">
-        <v>92</v>
-      </c>
-      <c r="C94"/>
-      <c r="F94" s="41"/>
-      <c r="G94" s="41"/>
-    </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="31">
-        <v>93</v>
-      </c>
-      <c r="C95" s="53" t="s">
-        <v>145</v>
-      </c>
-      <c r="F95" s="41"/>
-      <c r="G95" s="41"/>
-    </row>
-    <row r="96" spans="1:8" ht="90">
-      <c r="A96" s="31">
-        <v>94</v>
-      </c>
-      <c r="B96" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C96" t="s">
-        <v>146</v>
-      </c>
-      <c r="E96" s="50" t="s">
-        <v>220</v>
-      </c>
-      <c r="F96" s="41"/>
-      <c r="G96" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H96" s="43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" s="31">
-        <v>95</v>
-      </c>
-      <c r="C97"/>
-      <c r="D97" s="48"/>
-      <c r="E97" s="46"/>
-      <c r="F97" s="41"/>
-      <c r="G97" s="41"/>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" s="31">
-        <v>96</v>
-      </c>
-      <c r="C98" s="53" t="s">
-        <v>158</v>
-      </c>
-      <c r="D98" s="48"/>
-      <c r="E98" s="46"/>
-      <c r="F98" s="41"/>
-      <c r="G98" s="41"/>
-    </row>
-    <row r="99" spans="1:7" ht="360">
-      <c r="A99" s="31">
-        <v>97</v>
-      </c>
-      <c r="B99" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C99" t="s">
-        <v>148</v>
-      </c>
-      <c r="D99" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="E99" s="45" t="s">
-        <v>221</v>
-      </c>
-      <c r="F99" s="41"/>
-      <c r="G99" s="41"/>
-    </row>
-    <row r="100" spans="1:7" ht="150">
-      <c r="A100" s="31">
-        <v>98</v>
-      </c>
-      <c r="B100" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C100" t="s">
-        <v>151</v>
-      </c>
-      <c r="D100" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="E100" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="F100" s="41"/>
-      <c r="G100" s="41"/>
-    </row>
-    <row r="101" spans="1:7" ht="255">
-      <c r="A101" s="31">
-        <v>99</v>
-      </c>
-      <c r="B101" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C101" t="s">
-        <v>154</v>
-      </c>
-      <c r="D101" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="E101" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="F101" s="41"/>
-      <c r="G101" s="41"/>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" s="31">
-        <v>100</v>
-      </c>
-      <c r="B102" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C102" t="s">
-        <v>156</v>
-      </c>
-      <c r="D102" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="F102" s="41"/>
-      <c r="G102" s="41"/>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103" s="31">
-        <v>101</v>
-      </c>
-      <c r="C103"/>
-      <c r="F103" s="41"/>
-      <c r="G103" s="41"/>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" s="31">
-        <v>102</v>
-      </c>
-      <c r="C104" s="53" t="s">
-        <v>169</v>
-      </c>
-      <c r="F104" s="41"/>
-      <c r="G104" s="41"/>
-    </row>
-    <row r="105" spans="1:7" ht="75">
-      <c r="A105" s="31">
-        <v>103</v>
-      </c>
-      <c r="B105" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C105" t="s">
-        <v>170</v>
-      </c>
-      <c r="E105" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="F105" s="41"/>
-      <c r="G105" s="41"/>
-    </row>
-    <row r="106" spans="1:7" ht="150">
-      <c r="A106" s="31">
-        <v>104</v>
-      </c>
-      <c r="B106" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C106" t="s">
-        <v>5</v>
-      </c>
-      <c r="D106" s="39" t="s">
-        <v>193</v>
-      </c>
-      <c r="E106" s="45" t="s">
-        <v>224</v>
-      </c>
-      <c r="F106" s="41"/>
-      <c r="G106" s="41"/>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107" s="31">
-        <v>105</v>
-      </c>
-      <c r="C107"/>
-      <c r="F107" s="41"/>
-      <c r="G107" s="41"/>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="31">
-        <v>106</v>
-      </c>
-      <c r="C108" s="53" t="s">
-        <v>181</v>
-      </c>
-      <c r="F108" s="41"/>
-      <c r="G108" s="41"/>
-    </row>
-    <row r="109" spans="1:7" ht="45">
-      <c r="A109" s="31">
-        <v>107</v>
-      </c>
-      <c r="B109" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="C109" t="s">
-        <v>182</v>
-      </c>
-      <c r="D109" s="38" t="s">
-        <v>183</v>
-      </c>
-      <c r="E109" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="F109" s="41"/>
-      <c r="G109" s="41"/>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="A110" s="31">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" s="31">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112" s="31">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113" s="31">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" s="31">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" s="31">
-        <v>113</v>
-      </c>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="31">
+      <c r="A116" s="52">
         <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="31">
+      <c r="A117" s="52">
         <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="31">
+      <c r="A118" s="52">
         <v>116</v>
       </c>
     </row>
@@ -5189,7 +5062,7 @@
       <c r="A78" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B78" s="54" t="s">
+      <c r="B78" s="49" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5197,19 +5070,19 @@
       <c r="A79" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="54"/>
+      <c r="B79" s="49"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="54"/>
+      <c r="B80" s="49"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="54"/>
+      <c r="B81" s="49"/>
     </row>
     <row r="82" spans="1:3" ht="300">
       <c r="A82" s="19" t="s">

</xml_diff>

<commit_message>
Working on DownloadImage library.
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="240">
   <si>
     <t>UnFollowBusiness</t>
   </si>
@@ -1861,6 +1861,15 @@
   <si>
     <t>مرتبط با این تغییر، باگ شماره ۱۰۴ ایجاد شده است و نمیتوان
 تغییر محتوا را بررسی کرد.</t>
+  </si>
+  <si>
+    <t>6.1.2015</t>
+  </si>
+  <si>
+    <t>RegisterUser(method name: registerUser)</t>
+  </si>
+  <si>
+    <t>{"Error":{"ErrorCode":"Incorrect number of arguments supplied for call to method 'Boolean Equals(System.String, System.String, System.StringComparison)'"},"Result":"","SuccessStatus":false}</t>
   </si>
 </sst>
 </file>
@@ -2125,7 +2134,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2309,6 +2318,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2609,10 +2621,10 @@
   <dimension ref="A2:I118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D108" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4088,7 +4100,7 @@
       <c r="C80" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="64" t="s">
+      <c r="D80" s="65" t="s">
         <v>135</v>
       </c>
       <c r="F80" s="41"/>
@@ -4104,7 +4116,7 @@
       <c r="C81" t="s">
         <v>29</v>
       </c>
-      <c r="D81" s="64"/>
+      <c r="D81" s="65"/>
       <c r="F81" s="41"/>
       <c r="G81" s="41"/>
     </row>
@@ -4118,7 +4130,7 @@
       <c r="C82" t="s">
         <v>63</v>
       </c>
-      <c r="D82" s="64"/>
+      <c r="D82" s="65"/>
       <c r="F82" s="41"/>
       <c r="G82" s="41"/>
     </row>
@@ -4132,7 +4144,7 @@
       <c r="C83" t="s">
         <v>16</v>
       </c>
-      <c r="D83" s="64"/>
+      <c r="D83" s="65"/>
       <c r="F83" s="41"/>
       <c r="G83" s="41"/>
     </row>
@@ -4548,38 +4560,51 @@
       <c r="A111" s="31">
         <v>109</v>
       </c>
+      <c r="C111" s="52" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="31">
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C112" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="E112" s="64" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="31">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="31">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="31">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="31">
         <v>114</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C116" s="64"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="31">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="31">
         <v>116</v>
       </c>
@@ -5366,7 +5391,7 @@
       <c r="A78" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B78" s="65" t="s">
+      <c r="B78" s="66" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5374,19 +5399,19 @@
       <c r="A79" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="65"/>
+      <c r="B79" s="66"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="65"/>
+      <c r="B80" s="66"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="65"/>
+      <c r="B81" s="66"/>
     </row>
     <row r="82" spans="1:3" ht="300" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">

</xml_diff>

<commit_message>
bug haye webservice barresi mojadad shod va vaziate bug moshakhas shod!
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Android\Dev\4Soo\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Android\Dev\4Soo2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
-    <sheet name="Trash" sheetId="1" r:id="rId2"/>
+    <sheet name="WebServices With Bug" sheetId="5" r:id="rId2"/>
+    <sheet name="Trash" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="254">
   <si>
     <t>UnFollowBusiness</t>
   </si>
@@ -1187,13 +1188,6 @@
     <t>search: "arayeshgah"</t>
   </si>
   <si>
-    <t>I updated a post with these data:
-{"Picture":"","Description":"dhhhdh@dhdhs.com\n","Price":"100,000"
-,"HashTagList":"hdhd","Discount":"0","PostId":"3146","Code":"dhdhhhddh"
-,"Title":"poooooost update"}
-after updating I ran the GetPost webservice</t>
-  </si>
-  <si>
     <t>It returns the own user as friend</t>
   </si>
   <si>
@@ -1759,14 +1753,6 @@
   </si>
   <si>
     <t>sample URL:
-http://185.55.226.223:8081/bsn/getUserPost/2029/3146
-After update, GetPost returns the PostPictureId = 5512 which is NOT exist.
-It happens whenever I update a post.
-the result:
-{"Error":{"ErrorCode":null},"Result":"{\"UserId\":2029,\"BusinessId\":5059,\"PostId\":3146,\"UserName\":\"hamid1\",\"BusinessName\":null,\"Title\":\"poooooost update\",\"CreationDate\":\"0\",\"PostPictureId\":5512,\"BusinessProfilePictureId\":5508,\"Code\":\"dhdhhhddh\",\"Price\":\"100,000\",\"Comments\":\"[]\",\"Description\":\"dhhhdh@dhdhs.com\\n\",\"IsLiked\":false,\"IsShared\":false,\"IsReported\":false,\"HashTagList\":\"hdhd\"}","SuccessStatus":true}</t>
-  </si>
-  <si>
-    <t>sample URL:
 http://185.55.226.223:8081/bsn/getUserFriendList/2041
 "Result":"[{\"Id\":2041,\"UserId\":\"hamid10\",\"UserName\":\"hamid10\",\"UserProfilePictureId\":3258}
 ,{\"Id\":2041,\"UserId\":\"hamid10\",\"UserName\":\"hamid10\",\"UserProfilePictureId\":3258}]</t>
@@ -1884,12 +1870,130 @@
 Result:
 {"Error":{"ErrorCode":null},"Result":"{\"UserId\":2029,\"BusinessId\":3030,\"PostId\":4075,\"UserName\":\"hamid1\",\"BusinessName\":null,\"Title\":null,\"CreationDate\":\"20\",\"PostPictureId\":0,\"BusinessProfilePictureId\":5410,\"Code\":null,\"Price\":null,\"Comments\":\"[]\",\"Description\":null,\"IsLiked\":false,\"IsShared\":false,\"IsReported\":false,\"HashTagList\":null}","SuccessStatus":true}</t>
   </si>
+  <si>
+    <t>Not Confirmed!</t>
+  </si>
+  <si>
+    <t>returns error 08 just for this business</t>
+  </si>
+  <si>
+    <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserPost/2029/4075
+result:
+{"Error":{"ErrorCode":null},"Result":"{\"UserId\":2029,\"BusinessId\":3030,\"PostId\":4075,\"UserName\":\"hamid1\",\"BusinessName\":null,\"Title\":null,\"CreationDate\":\"162\",\"PostPictureId\":0,\"BusinessProfilePictureId\":5410,\"Code\":null,\"Price\":null,\"Comments\":\"[]\",\"Description\":null,\"IsLiked\":false,\"IsShared\":false,\"IsReported\":false,\"HashTagList\":null}","SuccessStatus":true}</t>
+  </si>
+  <si>
+    <t>Confirmed!
+تغییر اعمال شده است اما
+مقداری که برمیگردد
+اشتباه است
+برای url نمونه داده
+شده مقدار ۱۶۲ برمیگردد
+طبق رکوردهای شماره ۷۸ تا ۸۱
+قرار شده تاریخ با فرمت Date از سرور
+برگردد</t>
+  </si>
+  <si>
+    <t>registerBusiness</t>
+  </si>
+  <si>
+    <t>یک کد خطا برمیگرداند که گمان میکنم مربوط به تابع
+بررسی کننده یکتایی شناسه حرفی کسب و کار باشد</t>
+  </si>
+  <si>
+    <t>{"Error":{"ErrorCode":"Incorrect number of arguments
+supplied for call to method 'Boolean Equals(System.String
+, System.String, System.StringComparison)'"},"
+Result":"","SuccessStatus":false}</t>
+  </si>
+  <si>
+    <t>NOT Confirmed!
+با توجه به اینکه ثبت کسب
+وکار خطای رکورد شماره
+۱۱۱ از این فایل را
+برمیگرداند، امکان بررسی
+رفع شدن\نشدن این باگ وجود ندارد</t>
+  </si>
+  <si>
+    <t>NOT Confirmed!
+با توجه به وجود باگ شماره
+۱۰۳
+امکان بررسی رفع شدن \نشدن این باگ وجود ندارد</t>
+  </si>
+  <si>
+    <t>Confirmed!
+یکی از باگها حل شده
+باگ شماره یک که خود کاربر
+را به عنوان دوست
+برمیگرداند، هنوز وجود دارد
+و در رکورد شماره
+۹۸ گزارش شده است</t>
+  </si>
+  <si>
+    <t>تکراری</t>
+  </si>
+  <si>
+    <t>در متود ویرایش اطلاعات یک پست اگر تصویر
+پست (رشته) به صورت یک رشته تهی "" به سرور
+ارسال شود، فرض بر عدم تغییر تصویر فعلی پست در
+سرور است، در حالتی که وب سرویس مربوطه یک تصویر تهی برای آن پست ایجاد میکند و در دیتابیس قرار میدهد. 
+ویرایش اطلاعات پست با شناسه عددی ۳۱۵۸ بصورت گفته شده در بالا انجام شد
+سپس سرور یک تصویر تهی با شناسه عددی ۶۳۱۹
+را به آن اختصاص داد.</t>
+  </si>
+  <si>
+    <r>
+      <t>sample URL:
+http://185.55.226.223:8081/bsn/getUserPost/2029/3158
+{"Error":{"ErrorCode":null},"Result":"{\"UserId\":2029,\"BusinessId\":3034,\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PostId\":3158</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,\"UserName\":\"hamid1\",\"BusinessName\":null,\"Title\":\"hhggfg\",\"CreationDate\":\"433\",\"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PostPictureId\":6319</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,\"BusinessProfilePictureId\":5410,\"Code\":\"\",\"Price\":\"\",\"Comments\":\"[{\\\"CommentId\\\":3066,\\\"User_Id\\\":2029,\\\"UserId\\\":null,\\\"UserName\\\":\\\"حميد 1\\\",\\\"Text\\\":\\\"تلنذب\\\",\\\"ProfilePictureId\\\":2022}]\",\"Description\":\"tozihaat\",\"IsLiked\":false,\"IsShared\":false,\"IsReported\":true,\"HashTagList\":\"\"}","SuccessStatus":true}</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2016,8 +2120,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2103,8 +2214,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2121,8 +2237,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2146,8 +2277,9 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2342,10 +2474,29 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="2" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="4" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="9" builtinId="29"/>
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -2355,6 +2506,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="11" builtinId="10"/>
     <cellStyle name="Style 1" xfId="3"/>
     <cellStyle name="Style 2" xfId="4"/>
   </cellStyles>
@@ -2634,13 +2786,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I117"/>
+  <dimension ref="A2:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D111" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A115" sqref="A115:A119"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2658,7 +2810,7 @@
   <sheetData>
     <row r="2" spans="1:8" s="32" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
       <c r="A2" s="54" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>188</v>
@@ -2676,7 +2828,7 @@
         <v>187</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H2" s="37" t="s">
         <v>189</v>
@@ -2687,7 +2839,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2707,7 +2859,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -2735,16 +2887,16 @@
         <v>6</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F5" s="41" t="s">
         <v>159</v>
       </c>
       <c r="G5" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="63" t="s">
         <v>199</v>
-      </c>
-      <c r="H5" s="63" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2764,10 +2916,10 @@
         <v>159</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2787,10 +2939,10 @@
         <v>159</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H7" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2813,10 +2965,10 @@
         <v>160</v>
       </c>
       <c r="G8" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H8" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2854,10 +3006,10 @@
         <v>159</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H11" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="75">
@@ -2877,10 +3029,10 @@
         <v>159</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="75">
@@ -2888,7 +3040,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -2897,14 +3049,14 @@
         <v>12</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F13" s="41"/>
       <c r="G13" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H13" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H13" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="135">
@@ -2912,7 +3064,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -2921,14 +3073,14 @@
         <v>12</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H14" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H14" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="75">
@@ -2936,7 +3088,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -2945,14 +3097,14 @@
         <v>12</v>
       </c>
       <c r="E15" s="45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F15" s="41"/>
       <c r="G15" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H15" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H15" s="63" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2978,7 +3130,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
         <v>174</v>
@@ -3007,16 +3159,16 @@
         <v>98</v>
       </c>
       <c r="E19" s="45" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F19" s="41" t="s">
         <v>161</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45">
@@ -3036,10 +3188,10 @@
         <v>162</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H20" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45">
@@ -3059,10 +3211,10 @@
         <v>162</v>
       </c>
       <c r="G21" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H21" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="120">
@@ -3070,20 +3222,23 @@
         <v>20</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
       </c>
+      <c r="D22" s="39" t="s">
+        <v>242</v>
+      </c>
       <c r="E22" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F22" s="41"/>
       <c r="G22" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H22" s="44" t="s">
         <v>199</v>
-      </c>
-      <c r="H22" s="44" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -3129,20 +3284,20 @@
         <v>24</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C26" t="s">
         <v>36</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F26" s="41"/>
       <c r="G26" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H26" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H26" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="60">
@@ -3204,7 +3359,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C30" t="s">
         <v>43</v>
@@ -3214,10 +3369,10 @@
       </c>
       <c r="F30" s="41"/>
       <c r="G30" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H30" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H30" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="47" customFormat="1" ht="135">
@@ -3225,23 +3380,23 @@
         <v>29</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C31" s="58" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="62" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E31" s="59" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F31" s="57"/>
       <c r="G31" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H31" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I31" s="57"/>
     </row>
@@ -3263,12 +3418,12 @@
       <c r="F33" s="41"/>
       <c r="G33" s="41"/>
     </row>
-    <row r="34" spans="1:8" ht="165">
+    <row r="34" spans="1:8" ht="195">
       <c r="A34" s="31">
         <v>32</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
@@ -3277,14 +3432,14 @@
         <v>54</v>
       </c>
       <c r="E34" s="45" t="s">
-        <v>53</v>
+        <v>243</v>
       </c>
       <c r="F34" s="41"/>
       <c r="G34" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H34" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H34" s="71" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30">
@@ -3310,7 +3465,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
@@ -3323,10 +3478,10 @@
       </c>
       <c r="F36" s="41"/>
       <c r="G36" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H36" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H36" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -3386,12 +3541,12 @@
       </c>
       <c r="G40" s="41"/>
     </row>
-    <row r="41" spans="1:8" ht="45">
+    <row r="41" spans="1:8" ht="105">
       <c r="A41" s="31">
         <v>39</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C41" t="s">
         <v>59</v>
@@ -3399,12 +3554,13 @@
       <c r="D41" s="45" t="s">
         <v>60</v>
       </c>
+      <c r="E41" s="66"/>
       <c r="F41" s="41"/>
       <c r="G41" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H41" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H41" s="72" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="45">
@@ -3439,16 +3595,16 @@
         <v>68</v>
       </c>
       <c r="E43" s="45" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F43" s="41" t="s">
         <v>166</v>
       </c>
       <c r="G43" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="75">
@@ -3513,20 +3669,20 @@
         <v>45</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C47" t="s">
         <v>64</v>
       </c>
       <c r="E47" s="45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F47" s="41"/>
       <c r="G47" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H47" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H47" s="71" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="165">
@@ -3534,20 +3690,20 @@
         <v>46</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C48" t="s">
         <v>63</v>
       </c>
       <c r="E48" s="45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F48" s="41"/>
       <c r="G48" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H48" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H48" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3573,20 +3729,20 @@
         <v>49</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C51" t="s">
         <v>75</v>
       </c>
       <c r="E51" s="45" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F51" s="41"/>
       <c r="G51" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H51" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H51" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3594,7 +3750,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C52" t="s">
         <v>77</v>
@@ -3604,10 +3760,10 @@
       </c>
       <c r="F52" s="41"/>
       <c r="G52" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H52" s="70" t="s">
         <v>199</v>
-      </c>
-      <c r="H52" s="43" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3789,16 +3945,16 @@
         <v>95</v>
       </c>
       <c r="E63" s="45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F63" s="41" t="s">
         <v>168</v>
       </c>
       <c r="G63" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H63" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="45">
@@ -3824,7 +3980,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C65" t="s">
         <v>93</v>
@@ -3833,14 +3989,14 @@
         <v>190</v>
       </c>
       <c r="E65" s="45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F65" s="41"/>
       <c r="G65" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H65" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H65" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="60">
@@ -3848,7 +4004,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C66" t="s">
         <v>100</v>
@@ -3867,7 +4023,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C67" t="s">
         <v>103</v>
@@ -3960,20 +4116,20 @@
         <v>71</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C73" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F73" s="41"/>
       <c r="G73" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H73" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H73" s="73" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="75">
@@ -3981,7 +4137,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C74" t="s">
         <v>116</v>
@@ -3990,14 +4146,14 @@
         <v>117</v>
       </c>
       <c r="E74" s="45" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F74" s="41"/>
       <c r="G74" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H74" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="30">
@@ -4021,20 +4177,20 @@
         <v>74</v>
       </c>
       <c r="B76" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C76" t="s">
         <v>120</v>
       </c>
       <c r="E76" s="50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F76" s="41"/>
       <c r="G76" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H76" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H76" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="390">
@@ -4042,20 +4198,20 @@
         <v>75</v>
       </c>
       <c r="B77" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C77" t="s">
         <v>124</v>
       </c>
       <c r="E77" s="45" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F77" s="41"/>
       <c r="G77" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H77" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H77" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="75">
@@ -4063,23 +4219,23 @@
         <v>76</v>
       </c>
       <c r="B78" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C78" t="s">
         <v>124</v>
       </c>
       <c r="D78" s="45" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E78" s="45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F78" s="41"/>
       <c r="G78" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H78" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="90">
@@ -4087,23 +4243,23 @@
         <v>77</v>
       </c>
       <c r="B79" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C79" t="s">
         <v>124</v>
       </c>
       <c r="D79" s="45" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E79" s="45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F79" s="41"/>
       <c r="G79" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H79" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -4116,7 +4272,7 @@
       <c r="C80" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="66" t="s">
+      <c r="D80" s="67" t="s">
         <v>135</v>
       </c>
       <c r="F80" s="41"/>
@@ -4132,7 +4288,7 @@
       <c r="C81" t="s">
         <v>29</v>
       </c>
-      <c r="D81" s="66"/>
+      <c r="D81" s="67"/>
       <c r="F81" s="41"/>
       <c r="G81" s="41"/>
     </row>
@@ -4146,7 +4302,7 @@
       <c r="C82" t="s">
         <v>63</v>
       </c>
-      <c r="D82" s="66"/>
+      <c r="D82" s="67"/>
       <c r="F82" s="41"/>
       <c r="G82" s="41"/>
     </row>
@@ -4160,7 +4316,7 @@
       <c r="C83" t="s">
         <v>16</v>
       </c>
-      <c r="D83" s="66"/>
+      <c r="D83" s="67"/>
       <c r="F83" s="41"/>
       <c r="G83" s="41"/>
     </row>
@@ -4169,20 +4325,20 @@
         <v>82</v>
       </c>
       <c r="B84" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C84" t="s">
         <v>129</v>
       </c>
       <c r="E84" s="45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F84" s="41"/>
       <c r="G84" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H84" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H84" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="180">
@@ -4190,20 +4346,20 @@
         <v>83</v>
       </c>
       <c r="B85" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C85" t="s">
         <v>131</v>
       </c>
       <c r="E85" s="45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F85" s="41"/>
       <c r="G85" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H85" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H85" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -4211,7 +4367,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C86" t="s">
         <v>59</v>
@@ -4224,10 +4380,10 @@
       </c>
       <c r="F86" s="41"/>
       <c r="G86" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H86" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H86" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -4249,19 +4405,19 @@
       <c r="G88" s="41"/>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="31">
+      <c r="A89" s="74">
         <v>87</v>
       </c>
-      <c r="B89" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="B89" s="74" t="s">
+        <v>251</v>
+      </c>
+      <c r="C89" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="D89" s="39" t="s">
+      <c r="D89" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="E89" s="53" t="s">
+      <c r="E89" s="74" t="s">
         <v>78</v>
       </c>
       <c r="F89" s="41"/>
@@ -4291,20 +4447,20 @@
         <v>90</v>
       </c>
       <c r="B92" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C92" t="s">
         <v>7</v>
       </c>
       <c r="E92" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F92" s="41"/>
       <c r="G92" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H92" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H92" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="60">
@@ -4346,20 +4502,20 @@
         <v>94</v>
       </c>
       <c r="B96" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C96" t="s">
         <v>146</v>
       </c>
       <c r="E96" s="50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F96" s="41"/>
       <c r="G96" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="H96" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="H96" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4384,50 +4540,60 @@
       <c r="F98" s="41"/>
       <c r="G98" s="41"/>
     </row>
-    <row r="99" spans="1:8" ht="285">
+    <row r="99" spans="1:8" ht="240">
       <c r="A99" s="31">
         <v>97</v>
       </c>
       <c r="B99" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C99" t="s">
         <v>148</v>
       </c>
       <c r="D99" s="45" t="s">
-        <v>191</v>
+        <v>252</v>
       </c>
       <c r="E99" s="45" t="s">
-        <v>220</v>
+        <v>253</v>
       </c>
       <c r="F99" s="41"/>
-      <c r="G99" s="41"/>
+      <c r="G99" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H99" s="26" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="100" spans="1:8" ht="120">
       <c r="A100" s="31">
         <v>98</v>
       </c>
       <c r="B100" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C100" t="s">
         <v>151</v>
       </c>
       <c r="D100" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E100" s="45" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F100" s="41"/>
-      <c r="G100" s="41"/>
+      <c r="G100" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H100" s="26" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="101" spans="1:8" ht="255">
       <c r="A101" s="31">
         <v>99</v>
       </c>
       <c r="B101" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C101" t="s">
         <v>154</v>
@@ -4439,14 +4605,19 @@
         <v>78</v>
       </c>
       <c r="F101" s="41"/>
-      <c r="G101" s="41"/>
+      <c r="G101" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H101" s="26" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="102" spans="1:8" ht="105">
       <c r="A102" s="31">
         <v>100</v>
       </c>
       <c r="B102" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C102" t="s">
         <v>156</v>
@@ -4455,14 +4626,14 @@
         <v>157</v>
       </c>
       <c r="E102" s="45" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F102" s="41"/>
       <c r="G102" s="42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H102" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -4488,35 +4659,45 @@
         <v>103</v>
       </c>
       <c r="B105" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C105" t="s">
         <v>170</v>
       </c>
       <c r="E105" s="45" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F105" s="41"/>
-      <c r="G105" s="41"/>
+      <c r="G105" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H105" s="26" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="106" spans="1:8" ht="120">
       <c r="A106" s="31">
         <v>104</v>
       </c>
       <c r="B106" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C106" t="s">
         <v>5</v>
       </c>
       <c r="D106" s="39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E106" s="45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F106" s="41"/>
-      <c r="G106" s="41"/>
+      <c r="G106" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H106" s="26" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" s="31">
@@ -4541,7 +4722,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C109" t="s">
         <v>182</v>
@@ -4560,16 +4741,22 @@
         <v>108</v>
       </c>
       <c r="B110" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C110" t="s">
         <v>146</v>
       </c>
       <c r="D110" s="60" t="s">
+        <v>224</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="G110" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H110" s="26" t="s">
         <v>226</v>
-      </c>
-      <c r="E110" s="11" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4583,60 +4770,95 @@
     </row>
     <row r="112" spans="1:8">
       <c r="B112" s="52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C112" s="52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D112" s="52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E112" s="52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F112" s="52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G112" s="52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H112" s="52" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113" s="31">
         <v>109</v>
       </c>
       <c r="B113" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C113" s="39" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E113" s="64" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="195">
+        <v>237</v>
+      </c>
+      <c r="G113" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H113" s="26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="195">
       <c r="A114" s="31">
         <v>110</v>
       </c>
       <c r="B114" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C114" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="D114" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="E114" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D114" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="E114" s="45" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
-      <c r="C117" s="64"/>
+      <c r="G114" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H114" s="26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="90">
+      <c r="A115" s="31">
+        <v>111</v>
+      </c>
+      <c r="B115" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C115" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="D115" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="E115" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="G115" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H115" s="26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="C116" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4648,6 +4870,1882 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="66" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="66" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" style="66" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="66" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="66" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" s="32" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A2" s="54" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="75.75" thickTop="1">
+      <c r="A3" s="31">
+        <f>TODO!A13</f>
+        <v>11</v>
+      </c>
+      <c r="B3" s="36" t="str">
+        <f>TODO!B13</f>
+        <v>bug</v>
+      </c>
+      <c r="C3" t="str">
+        <f>TODO!C13</f>
+        <v>DeletePost</v>
+      </c>
+      <c r="D3" s="45" t="str">
+        <f>TODO!D13</f>
+        <v>Error</v>
+      </c>
+      <c r="E3" s="50" t="str">
+        <f>TODO!E13</f>
+        <v>sample url:
+http://185.55.226.223:8081/bsn/deletePost/2/52
+{"Error":{"ErrorCode":"10"},"Result":"False","SuccessStatus":false}</v>
+      </c>
+      <c r="F3" s="41">
+        <f>TODO!F13</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="42" t="str">
+        <f>TODO!G13</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H3" s="69" t="str">
+        <f>TODO!H13</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="135">
+      <c r="A4" s="31">
+        <f>TODO!A14</f>
+        <v>12</v>
+      </c>
+      <c r="B4" s="36" t="str">
+        <f>TODO!B14</f>
+        <v>bug</v>
+      </c>
+      <c r="C4" t="str">
+        <f>TODO!C14</f>
+        <v>GetBusinessContactInfo</v>
+      </c>
+      <c r="D4" s="45" t="str">
+        <f>TODO!D14</f>
+        <v>Error</v>
+      </c>
+      <c r="E4" s="45" t="str">
+        <f>TODO!E14</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getBusinessContactInfo/2
+returns website as null
+{"Phone":"www.google.com","Email":"sd@xxx.com","Website":null,"Mobile":"11111111","Latitude":35.6975323181562,"WorkTimeClose":"17:00","Longitude":51.3911837339401,"WorkTimeOpen":"08:00"}</v>
+      </c>
+      <c r="F4" s="41">
+        <f>TODO!F14</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="42" t="str">
+        <f>TODO!G14</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H4" s="69" t="str">
+        <f>TODO!H14</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75">
+      <c r="A5" s="31">
+        <f>TODO!A15</f>
+        <v>13</v>
+      </c>
+      <c r="B5" s="36" t="str">
+        <f>TODO!B15</f>
+        <v>bug</v>
+      </c>
+      <c r="C5" t="str">
+        <f>TODO!C15</f>
+        <v>GetBlockedUsers</v>
+      </c>
+      <c r="D5" s="45" t="str">
+        <f>TODO!D15</f>
+        <v>Error</v>
+      </c>
+      <c r="E5" s="45" t="str">
+        <f>TODO!E15</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getBlockedUsersList/2
+Endpoint not found.</v>
+      </c>
+      <c r="F5" s="41">
+        <f>TODO!F15</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="42" t="str">
+        <f>TODO!G15</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H5" s="63" t="str">
+        <f>TODO!H15</f>
+        <v>Not Confirmed!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="31">
+        <f>TODO!A17</f>
+        <v>15</v>
+      </c>
+      <c r="B6" s="31">
+        <f>TODO!B17</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="52" t="str">
+        <f>TODO!C17</f>
+        <v>4.7.2015</v>
+      </c>
+      <c r="D6" s="66">
+        <f>TODO!D17</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="66">
+        <f>TODO!E17</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="41">
+        <f>TODO!F17</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="41">
+        <f>TODO!G17</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="66">
+        <f>TODO!H17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="120">
+      <c r="A7" s="31">
+        <f>TODO!A22</f>
+        <v>20</v>
+      </c>
+      <c r="B7" s="36" t="str">
+        <f>TODO!B22</f>
+        <v>bug</v>
+      </c>
+      <c r="C7" t="str">
+        <f>TODO!C22</f>
+        <v>getBusinessContactInfo</v>
+      </c>
+      <c r="D7" s="66" t="str">
+        <f>TODO!D22</f>
+        <v>returns error 08 just for this business</v>
+      </c>
+      <c r="E7" s="50" t="str">
+        <f>TODO!E22</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getBusinessContactInfo/1
+{"Error":{"ErrorCode":"08"},"Result":"","SuccessStatus":false}: it is a Get not Post
+It works fiine for all businesses except id = 1</v>
+      </c>
+      <c r="F7" s="41">
+        <f>TODO!F22</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="42" t="str">
+        <f>TODO!G22</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H7" s="44" t="str">
+        <f>TODO!H22</f>
+        <v>NOT Confirmed!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="31">
+        <f>TODO!A25</f>
+        <v>23</v>
+      </c>
+      <c r="B8" s="31">
+        <f>TODO!B25</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="52" t="str">
+        <f>TODO!C25</f>
+        <v>4.11.2015</v>
+      </c>
+      <c r="D8" s="49">
+        <f>TODO!D25</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="66">
+        <f>TODO!E25</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="41">
+        <f>TODO!F25</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="41">
+        <f>TODO!G25</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="66">
+        <f>TODO!H25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="255">
+      <c r="A9" s="31">
+        <f>TODO!A26</f>
+        <v>24</v>
+      </c>
+      <c r="B9" s="36" t="str">
+        <f>TODO!B26</f>
+        <v>bug</v>
+      </c>
+      <c r="C9" t="str">
+        <f>TODO!C26</f>
+        <v>getUserHomeInfo</v>
+      </c>
+      <c r="D9" s="66">
+        <f>TODO!D26</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="50" t="str">
+        <f>TODO!E26</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserHomeInfo/2023/2019
+There is no record in db for user.id=2023 and user.id=2019 but the FriendshipRelationStatusCode is 4 that is wrong. It should be 2 (not friend)
+{"Error":{"ErrorCode":null},"Result":"{\"Name\":\"abkaveh\",\"AboutMe\":null,\"ProfilePictureId\
+":3189,\"CoverPictureId\":0,\"FriendRequestNumber\":0,\"FollowedBusinessNumber\":0,
+\"FriendsNumber\":0,\"ReviewsNumber\":0,\"Permission\":\"{\\\"Friends\\\":true,\\\"Reviews
+\\\":true,\\\"FollowedBusinesses\\\":true}\",\"FriendshipRelationStatusCode\":4,\"Businesses\
+":null,\"UserId\":\"ab.kaveh\"}","SuccessStatus":true}</v>
+      </c>
+      <c r="F9" s="41">
+        <f>TODO!F26</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="42" t="str">
+        <f>TODO!G26</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H9" s="69" t="str">
+        <f>TODO!H26</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60">
+      <c r="A10" s="31">
+        <f>TODO!A30</f>
+        <v>28</v>
+      </c>
+      <c r="B10" s="36" t="str">
+        <f>TODO!B30</f>
+        <v>bug</v>
+      </c>
+      <c r="C10" t="str">
+        <f>TODO!C30</f>
+        <v>reviewBusiness</v>
+      </c>
+      <c r="D10" s="45" t="str">
+        <f>TODO!D30</f>
+        <v>If  user reviewed  business before, it doesn't insert new record that is correct  but returns success=true. It should returns success=false with error</v>
+      </c>
+      <c r="E10" s="66">
+        <f>TODO!E30</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="41">
+        <f>TODO!F30</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="42" t="str">
+        <f>TODO!G30</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H10" s="69" t="str">
+        <f>TODO!H30</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="135">
+      <c r="A11" s="61">
+        <f>TODO!A31</f>
+        <v>29</v>
+      </c>
+      <c r="B11" s="36" t="str">
+        <f>TODO!B31</f>
+        <v>bug</v>
+      </c>
+      <c r="C11" s="58" t="str">
+        <f>TODO!C31</f>
+        <v>getAllCommentNotifications</v>
+      </c>
+      <c r="D11" s="62" t="str">
+        <f>TODO!D31</f>
+        <v>این سرویس قرار بوده است تمام کامنتهای تمام پستهای تمام کسب و کارهای یک کاربر را برگرداند.
+اطلاعاتی شامل:
+شناسه پست هر کامنت
+شناسه کاربری که کامنت گذاشته
+و ... که مربوط به هر کامنت است.
+قرار است مکانیزم گرفتن نوتیفیکیشن از سرور تغییر کند، فکر میکنم بهتر هست در مورد بررسی این رکورد با آقای پاکزاد هماهنگ کنید.</v>
+      </c>
+      <c r="E11" s="59" t="str">
+        <f>TODO!E31</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getAllCommentNotifications/3/0/20
+It returns empty result
+{"Error":{"ErrorCode":null},"Result":"[]","SuccessStatus":true}</v>
+      </c>
+      <c r="F11" s="57">
+        <f>TODO!F31</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="42" t="str">
+        <f>TODO!G31</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H11" s="26" t="str">
+        <f>TODO!H31</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="31">
+        <f>TODO!A33</f>
+        <v>31</v>
+      </c>
+      <c r="B12" s="31">
+        <f>TODO!B33</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="52" t="str">
+        <f>TODO!C33</f>
+        <v>4.12.2015</v>
+      </c>
+      <c r="D12" s="66">
+        <f>TODO!D33</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="66">
+        <f>TODO!E33</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="41">
+        <f>TODO!F33</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="41">
+        <f>TODO!G33</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="66">
+        <f>TODO!H33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="195">
+      <c r="A13" s="31">
+        <f>TODO!A34</f>
+        <v>32</v>
+      </c>
+      <c r="B13" s="36" t="str">
+        <f>TODO!B34</f>
+        <v>bug</v>
+      </c>
+      <c r="C13" t="str">
+        <f>TODO!C34</f>
+        <v>GetPost</v>
+      </c>
+      <c r="D13" s="45" t="str">
+        <f>TODO!D34</f>
+        <v>Error
+creationDate should be an int not String
+it should be like getUserPost webservice</v>
+      </c>
+      <c r="E13" s="45" t="str">
+        <f>TODO!E34</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserPost/2029/4075
+result:
+{"Error":{"ErrorCode":null},"Result":"{\"UserId\":2029,\"BusinessId\":3030,\"PostId\":4075,\"UserName\":\"hamid1\",\"BusinessName\":null,\"Title\":null,\"CreationDate\":\"162\",\"PostPictureId\":0,\"BusinessProfilePictureId\":5410,\"Code\":null,\"Price\":null,\"Comments\":\"[]\",\"Description\":null,\"IsLiked\":false,\"IsShared\":false,\"IsReported\":false,\"HashTagList\":null}","SuccessStatus":true}</v>
+      </c>
+      <c r="F13" s="41">
+        <f>TODO!F34</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="42" t="str">
+        <f>TODO!G34</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H13" s="71" t="str">
+        <f>TODO!H34</f>
+        <v>Confirmed!
+تغییر اعمال شده است اما
+مقداری که برمیگردد
+اشتباه است
+برای url نمونه داده
+شده مقدار ۱۶۲ برمیگردد
+طبق رکوردهای شماره ۷۸ تا ۸۱
+قرار شده تاریخ با فرمت Date از سرور
+برگردد</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="150">
+      <c r="A14" s="31">
+        <f>TODO!A36</f>
+        <v>34</v>
+      </c>
+      <c r="B14" s="36" t="str">
+        <f>TODO!B36</f>
+        <v>bug</v>
+      </c>
+      <c r="C14" t="str">
+        <f>TODO!C36</f>
+        <v>GetBusinessProfileInfo:</v>
+      </c>
+      <c r="D14" s="66" t="str">
+        <f>TODO!D36</f>
+        <v>there is no website:String in output</v>
+      </c>
+      <c r="E14" s="45" t="str">
+        <f>TODO!E36</f>
+        <v xml:space="preserve">
+{"LocationLongitude":"51.3911837339401","Phone":"555555555","Description":"ddddddddddd","HashTagList":"","CoverPicture":"","WorkTimeClose":"17:00","WorkDays":"1,5,6,7","ProfilePicture":"2022","City":"تهران","Name":"lk2222","Category":"cloth","Email":"sd@xxx.com","State":"تهران","Address":"آدرس","SubCategory":"men cloth","Mobile":"11111111","LocationLatitude":"35.6975323181562","WorkTimeOpen":"08:00"}</v>
+      </c>
+      <c r="F14" s="41">
+        <f>TODO!F36</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="42" t="str">
+        <f>TODO!G36</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H14" s="69" t="str">
+        <f>TODO!H36</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="31">
+        <f>TODO!A39</f>
+        <v>37</v>
+      </c>
+      <c r="B15" s="31">
+        <f>TODO!B39</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="52" t="str">
+        <f>TODO!C39</f>
+        <v>4.18.2015</v>
+      </c>
+      <c r="D15" s="66">
+        <f>TODO!D39</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="66">
+        <f>TODO!E39</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="41">
+        <f>TODO!F39</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="41">
+        <f>TODO!G39</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="66">
+        <f>TODO!H39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="105">
+      <c r="A16" s="31">
+        <f>TODO!A41</f>
+        <v>39</v>
+      </c>
+      <c r="B16" s="36" t="str">
+        <f>TODO!B41</f>
+        <v>bug</v>
+      </c>
+      <c r="C16" t="str">
+        <f>TODO!C41</f>
+        <v>RegisterBusiness</v>
+      </c>
+      <c r="D16" s="45" t="str">
+        <f>TODO!D41</f>
+        <v>business.id:String must be unique. User shouldn't be able to register
+many businesses with one buisness.id</v>
+      </c>
+      <c r="E16" s="66">
+        <f>TODO!E41</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="41">
+        <f>TODO!F41</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="42" t="str">
+        <f>TODO!G41</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H16" s="72" t="str">
+        <f>TODO!H41</f>
+        <v>NOT Confirmed!
+با توجه به اینکه ثبت کسب
+وکار خطای رکورد شماره
+۱۱۱ از این فایل را
+برمیگرداند، امکان بررسی
+رفع شدن\نشدن این باگ وجود ندارد</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="225">
+      <c r="A17" s="31">
+        <f>TODO!A47</f>
+        <v>45</v>
+      </c>
+      <c r="B17" s="36" t="str">
+        <f>TODO!B47</f>
+        <v>bug</v>
+      </c>
+      <c r="C17" t="str">
+        <f>TODO!C47</f>
+        <v>GetBusinessReviews</v>
+      </c>
+      <c r="D17" s="66">
+        <f>TODO!D47</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="45" t="str">
+        <f>TODO!E47</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getBusinessReviews/3030/0/20
+wrong usreId:int. Users how reviewed the business are userId:2029 and userId:2030 not userId:1012 and userId:1014
+{"Error":{"ErrorCode":null},"Result":"[{\"Rate\":5,\"ReviewId\":1014,\"UserId\":1014,\"UserName\":\"hamid2\",\"UserProfilePictureId\":3247,\"Text\":\"بسیار هم عالیه\",\"Like\":0},{\"Rate\":5,\"ReviewId\":1012,\"UserId\":1012,\"UserName\":\"hamid1\",\"UserProfilePictureId\":0,\"Text\":\"خیلی خوبه\",\"Like\":0}]","SuccessStatus":true}</v>
+      </c>
+      <c r="F17" s="41">
+        <f>TODO!F47</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="42" t="str">
+        <f>TODO!G47</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H17" s="71" t="str">
+        <f>TODO!H47</f>
+        <v>NOT Confirmed!
+با توجه به وجود باگ شماره
+۱۰۳
+امکان بررسی رفع شدن \نشدن این باگ وجود ندارد</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="165">
+      <c r="A18" s="31">
+        <f>TODO!A48</f>
+        <v>46</v>
+      </c>
+      <c r="B18" s="36" t="str">
+        <f>TODO!B48</f>
+        <v>bug</v>
+      </c>
+      <c r="C18" t="str">
+        <f>TODO!C48</f>
+        <v>GetWallPosts</v>
+      </c>
+      <c r="D18" s="66">
+        <f>TODO!D48</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="45" t="str">
+        <f>TODO!E48</f>
+        <v xml:space="preserve">sample URL:
+http://185.55.226.223:8081/bsn/getWallPosts/2030/0/20
+the user didn't share the following  posts but "IsLiked" is true for all of them
+….\"PostId\":1086…..
+…."PostId\":1085,…..
+…..\"PostId\":1084,….
+…..\"PostId\":1083,…..
+</v>
+      </c>
+      <c r="F18" s="41">
+        <f>TODO!F48</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="42" t="str">
+        <f>TODO!G48</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H18" s="69" t="str">
+        <f>TODO!H48</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="31">
+        <f>TODO!A50</f>
+        <v>48</v>
+      </c>
+      <c r="B19" s="31">
+        <f>TODO!B50</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="52" t="str">
+        <f>TODO!C50</f>
+        <v>4.19.2015</v>
+      </c>
+      <c r="D19" s="66">
+        <f>TODO!D50</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="66">
+        <f>TODO!E50</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="41">
+        <f>TODO!F50</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="41">
+        <f>TODO!G50</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="66">
+        <f>TODO!H50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="90">
+      <c r="A20" s="31">
+        <f>TODO!A51</f>
+        <v>49</v>
+      </c>
+      <c r="B20" s="36" t="str">
+        <f>TODO!B51</f>
+        <v>bug</v>
+      </c>
+      <c r="C20" t="str">
+        <f>TODO!C51</f>
+        <v>CommentOnPost</v>
+      </c>
+      <c r="D20" s="66">
+        <f>TODO!D51</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="45" t="str">
+        <f>TODO!E51</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/commentOnPost/2019/1058/test
+The userId=2019 is blocked by the post's owner (businessId=2) but he can send comment on post</v>
+      </c>
+      <c r="F20" s="41">
+        <f>TODO!F51</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="42" t="str">
+        <f>TODO!G51</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H20" s="69" t="str">
+        <f>TODO!H51</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="31">
+        <f>TODO!A52</f>
+        <v>50</v>
+      </c>
+      <c r="B21" s="36" t="str">
+        <f>TODO!B52</f>
+        <v>bug</v>
+      </c>
+      <c r="C21" t="str">
+        <f>TODO!C52</f>
+        <v>UpdateUserProfile</v>
+      </c>
+      <c r="D21" s="66" t="str">
+        <f>TODO!D52</f>
+        <v>Error 10</v>
+      </c>
+      <c r="E21" s="66">
+        <f>TODO!E52</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="41">
+        <f>TODO!F52</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="42" t="str">
+        <f>TODO!G52</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H21" s="70" t="str">
+        <f>TODO!H52</f>
+        <v>NOT Confirmed!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="31">
+        <f>TODO!A54</f>
+        <v>52</v>
+      </c>
+      <c r="B22" s="31">
+        <f>TODO!B54</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="52" t="str">
+        <f>TODO!C54</f>
+        <v>4.22.2015</v>
+      </c>
+      <c r="D22" s="66">
+        <f>TODO!D54</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="66">
+        <f>TODO!E54</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="41">
+        <f>TODO!F54</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="41">
+        <f>TODO!G54</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="66">
+        <f>TODO!H54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="105">
+      <c r="A23" s="31">
+        <f>TODO!A65</f>
+        <v>63</v>
+      </c>
+      <c r="B23" s="36" t="str">
+        <f>TODO!B65</f>
+        <v>bug</v>
+      </c>
+      <c r="C23" t="str">
+        <f>TODO!C65</f>
+        <v>SearchBusinessesLocation</v>
+      </c>
+      <c r="D23" s="45" t="str">
+        <f>TODO!D65</f>
+        <v>search: "arayeshgah"</v>
+      </c>
+      <c r="E23" s="45" t="str">
+        <f>TODO!E65</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/searchBusinessByLocation/hamidfastfood/11/35.84993291495611/51.66665095835924/0/20
+It doesn’t return  result while there is a business with businessId: "arayeshgah"</v>
+      </c>
+      <c r="F23" s="41">
+        <f>TODO!F65</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="42" t="str">
+        <f>TODO!G65</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H23" s="69" t="str">
+        <f>TODO!H65</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="31">
+        <f>TODO!A72</f>
+        <v>70</v>
+      </c>
+      <c r="B24" s="31">
+        <f>TODO!B72</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="52" t="str">
+        <f>TODO!C72</f>
+        <v>4.25.2015</v>
+      </c>
+      <c r="D24" s="66">
+        <f>TODO!D72</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="66">
+        <f>TODO!E72</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="41">
+        <f>TODO!F72</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="41">
+        <f>TODO!G72</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="66">
+        <f>TODO!H72</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="195">
+      <c r="A25" s="31">
+        <f>TODO!A73</f>
+        <v>71</v>
+      </c>
+      <c r="B25" s="36" t="str">
+        <f>TODO!B73</f>
+        <v>bug</v>
+      </c>
+      <c r="C25" t="str">
+        <f>TODO!C73</f>
+        <v>GetUserFriends</v>
+      </c>
+      <c r="D25" s="66">
+        <f>TODO!D73</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="45" t="str">
+        <f>TODO!E73</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendList/2029
+1. Returns the own user as his friend
+2. Returns some user's profilePictureId = 0
+{\"Id\":2036,\"UserId\":\"hamid5\",\"UserName\":\"hamid5\",\"UserProfilePictureId\":0},{\"Id\":2037,\"UserId\":\"hamid6\",\"UserName\":\"hamid6\",\"UserProfilePictureId\":0},{\"Id\":2029,\"UserId\":\"hamid1\",\"UserName\":\"hamid1\",\"UserProfilePictureId\":4313}</v>
+      </c>
+      <c r="F25" s="41">
+        <f>TODO!F73</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="42" t="str">
+        <f>TODO!G73</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H25" s="73" t="str">
+        <f>TODO!H73</f>
+        <v>Confirmed!
+یکی از باگها حل شده
+باگ شماره یک که خود کاربر
+را به عنوان دوست
+برمیگرداند، هنوز وجود دارد
+و در رکورد شماره
+۹۸ گزارش شده است</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="75">
+      <c r="A26" s="31">
+        <f>TODO!A74</f>
+        <v>72</v>
+      </c>
+      <c r="B26" s="36" t="str">
+        <f>TODO!B74</f>
+        <v>bug</v>
+      </c>
+      <c r="C26" t="str">
+        <f>TODO!C74</f>
+        <v>Post webserices</v>
+      </c>
+      <c r="D26" s="66" t="str">
+        <f>TODO!D74</f>
+        <v>if json length (image length) be more than 100,000 it returns HTTP/1.1 400 Bad Request</v>
+      </c>
+      <c r="E26" s="45" t="str">
+        <f>TODO!E74</f>
+        <v>در صورتی که پس از تبدیل عکس به استرینگ و قرار دادن
+محتوای آن در JSON، اندازه JSON از حدی بزرگتر شود، در ارسال آن به سرور، سرور خطای گفته شده را برمیگرداند.
+این عملکرد بر روی کامپیوتر شما به صورت محلی تست شد و اوکی بود.</v>
+      </c>
+      <c r="F26" s="41">
+        <f>TODO!F74</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="42" t="str">
+        <f>TODO!G74</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H26" s="26" t="str">
+        <f>TODO!H74</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="90">
+      <c r="A27" s="31">
+        <f>TODO!A76</f>
+        <v>74</v>
+      </c>
+      <c r="B27" s="36" t="str">
+        <f>TODO!B76</f>
+        <v>bug</v>
+      </c>
+      <c r="C27" t="str">
+        <f>TODO!C76</f>
+        <v>CancelShare</v>
+      </c>
+      <c r="D27" s="66">
+        <f>TODO!D76</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="50" t="str">
+        <f>TODO!E76</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/cancelShare/3/27
+{"Error":{"ErrorCode":"Value cannot be null.\u000d\u000aParameter name: entity"},"Result":"False","SuccessStatus":false}</v>
+      </c>
+      <c r="F27" s="41">
+        <f>TODO!F76</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="42" t="str">
+        <f>TODO!G76</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H27" s="69" t="str">
+        <f>TODO!H76</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="390">
+      <c r="A28" s="31">
+        <f>TODO!A77</f>
+        <v>75</v>
+      </c>
+      <c r="B28" s="36" t="str">
+        <f>TODO!B77</f>
+        <v>bug</v>
+      </c>
+      <c r="C28" t="str">
+        <f>TODO!C77</f>
+        <v>getWallPosts</v>
+      </c>
+      <c r="D28" s="66">
+        <f>TODO!D77</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="45" t="str">
+        <f>TODO!E77</f>
+        <v xml:space="preserve">It returns UserId=1 while the userId=3
+sample URL:
+http://185.55.226.223:8081/bsn/getWallPosts/3/0/20
+It returns IsLiked = true for PostId=27 while it is false
+\"UserId\":1,
+\"CommentNumber\":22,
+\"LikeNumber\":0,
+\"ShareNumber\":0,
+\"UserName\":\"sss\",
+\"PostId\":27,
+\"PostTypeId\":1,
+\"BusinessId\":1,
+\"BusinessUserName\":\"dkad\",
+\"CreationDate\":\"1821\",
+\"Title\":\"post3\",
+\"PostPictureId\":2022,
+\"BusinessProfilePictureId\":2022,
+\"Code\":\"5214\",
+\"Description\":\"des3\",
+\"Price\":\"123\",
+\"IsLiked\":true,
+</v>
+      </c>
+      <c r="F28" s="41">
+        <f>TODO!F77</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="42" t="str">
+        <f>TODO!G77</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H28" s="69" t="str">
+        <f>TODO!H77</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="75">
+      <c r="A29" s="31">
+        <f>TODO!A78</f>
+        <v>76</v>
+      </c>
+      <c r="B29" s="36" t="str">
+        <f>TODO!B78</f>
+        <v>bug</v>
+      </c>
+      <c r="C29" t="str">
+        <f>TODO!C78</f>
+        <v>getWallPosts</v>
+      </c>
+      <c r="D29" s="45" t="str">
+        <f>TODO!D78</f>
+        <v>سرور قرار است بر اساس نمونه URL داده شده،‌
+ ۲۰ پست را برای نمایش برگرداند اما در عمل
+تعداد بیشتری پست برمیگرداند</v>
+      </c>
+      <c r="E29" s="45" t="str">
+        <f>TODO!E78</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getWallPosts/2029/0/20
+returns 30 items instead of 20 (limitation)</v>
+      </c>
+      <c r="F29" s="41">
+        <f>TODO!F78</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="42" t="str">
+        <f>TODO!G78</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H29" s="26" t="str">
+        <f>TODO!H78</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="90">
+      <c r="A30" s="31">
+        <f>TODO!A79</f>
+        <v>77</v>
+      </c>
+      <c r="B30" s="36" t="str">
+        <f>TODO!B79</f>
+        <v>bug</v>
+      </c>
+      <c r="C30" t="str">
+        <f>TODO!C79</f>
+        <v>getWallPosts</v>
+      </c>
+      <c r="D30" s="45" t="str">
+        <f>TODO!D79</f>
+        <v>در پاسخی که از طرف سرور برمیگردد، 
+بعضی پست های تکراری وجود دارد.
+مثلا برای URL نمونه داده شده، پست با شناسه 1079
+در پاسخ سرور دوبار تکرار شده است.</v>
+      </c>
+      <c r="E30" s="45" t="str">
+        <f>TODO!E79</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getWallPosts/2029/0/20
+returns some items twice like postId=1079  and postId=1068</v>
+      </c>
+      <c r="F30" s="41">
+        <f>TODO!F79</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="42" t="str">
+        <f>TODO!G79</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H30" s="26" t="str">
+        <f>TODO!H79</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="225">
+      <c r="A31" s="31">
+        <f>TODO!A84</f>
+        <v>82</v>
+      </c>
+      <c r="B31" s="36" t="str">
+        <f>TODO!B84</f>
+        <v>bug</v>
+      </c>
+      <c r="C31" t="str">
+        <f>TODO!C84</f>
+        <v>getUserFriendRequestList</v>
+      </c>
+      <c r="D31" s="66">
+        <f>TODO!D84</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="45" t="str">
+        <f>TODO!E84</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendRequestList/2029
+It returns all UserProfilePictureId = 2022
+[{\"Id\":2034,\"UserId\":\"hamid3\",\"UserName\":\"hamid3\",\"UserProfilePictureId\":2022},{\"Id\":2036,\"UserId\":\"hamid5\",\"UserName\":\"hamid5\",\"UserProfilePictureId\":2022},{\"Id\":2037,\"UserId\":\"hamid6\",\"UserName\":\"hamid6\",\"UserProfilePictureId\":2022},{\"Id\":4066,\"UserId\":\"tessst\",\"UserName\":\"تست\",\"UserProfilePictureId\":2022},{\"Id\":3,\"UserId\":\"aliUserId\",\"UserName\":\"sss\",\"UserProfilePictureId\":2022}]</v>
+      </c>
+      <c r="F31" s="41">
+        <f>TODO!F84</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="42" t="str">
+        <f>TODO!G84</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H31" s="69" t="str">
+        <f>TODO!H84</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="180">
+      <c r="A32" s="31">
+        <f>TODO!A85</f>
+        <v>83</v>
+      </c>
+      <c r="B32" s="36" t="str">
+        <f>TODO!B85</f>
+        <v>bug</v>
+      </c>
+      <c r="C32" t="str">
+        <f>TODO!C85</f>
+        <v>getUserFriendList</v>
+      </c>
+      <c r="D32" s="66">
+        <f>TODO!D85</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="45" t="str">
+        <f>TODO!E85</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendList/2029
+It returns all UserProfilePictureId = 2022
+[{\"Id\":2034,\"UserId\":\"hamid3\",\"UserName\":\"hamid3\",\"UserProfilePictureId\":2022},{\"Id\":2036,\"UserId\":\"hamid5\",\"UserName\":\"hamid5\",\"UserProfilePictureId\":2022},{\"Id\":2037,\"UserId\":\"hamid6\",\"UserName\":\"hamid6\",\"UserProfilePictureId\":2022}]</v>
+      </c>
+      <c r="F32" s="41">
+        <f>TODO!F85</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="42" t="str">
+        <f>TODO!G85</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H32" s="69" t="str">
+        <f>TODO!H85</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="31">
+        <f>TODO!A86</f>
+        <v>84</v>
+      </c>
+      <c r="B33" s="36" t="str">
+        <f>TODO!B86</f>
+        <v>bug</v>
+      </c>
+      <c r="C33" t="str">
+        <f>TODO!C86</f>
+        <v>RegisterBusiness</v>
+      </c>
+      <c r="D33" s="66" t="str">
+        <f>TODO!D86</f>
+        <v>Sample in file which is attached to the email.</v>
+      </c>
+      <c r="E33" s="66" t="str">
+        <f>TODO!E86</f>
+        <v>returns ""</v>
+      </c>
+      <c r="F33" s="41">
+        <f>TODO!F86</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="42" t="str">
+        <f>TODO!G86</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H33" s="69" t="str">
+        <f>TODO!H86</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="31">
+        <f>TODO!A91</f>
+        <v>89</v>
+      </c>
+      <c r="B34" s="31">
+        <f>TODO!B91</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="52" t="str">
+        <f>TODO!C91</f>
+        <v>5.18.2015</v>
+      </c>
+      <c r="D34" s="66">
+        <f>TODO!D91</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="66">
+        <f>TODO!E91</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="41">
+        <f>TODO!F91</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="41">
+        <f>TODO!G91</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="66">
+        <f>TODO!H91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="105">
+      <c r="A35" s="31">
+        <f>TODO!A92</f>
+        <v>90</v>
+      </c>
+      <c r="B35" s="36" t="str">
+        <f>TODO!B92</f>
+        <v>bug</v>
+      </c>
+      <c r="C35" t="str">
+        <f>TODO!C92</f>
+        <v>GetUserFriends</v>
+      </c>
+      <c r="D35" s="66">
+        <f>TODO!D92</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="50" t="str">
+        <f>TODO!E92</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendList/2034
+The result should be like this: Id=2029 &amp; UserId = "hamid1"
+[{\"Id\":2034,\"UserId\":\"hamid3\",\"UserName\":\"hamid3\",\"UserProfilePictureId\":2022}]</v>
+      </c>
+      <c r="F35" s="41">
+        <f>TODO!F92</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="42" t="str">
+        <f>TODO!G92</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H35" s="69" t="str">
+        <f>TODO!H92</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="31">
+        <f>TODO!A95</f>
+        <v>93</v>
+      </c>
+      <c r="B36" s="31">
+        <f>TODO!B95</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="52" t="str">
+        <f>TODO!C95</f>
+        <v>5.19.2015</v>
+      </c>
+      <c r="D36" s="66">
+        <f>TODO!D95</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="66">
+        <f>TODO!E95</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="41">
+        <f>TODO!F95</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="41">
+        <f>TODO!G95</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="66">
+        <f>TODO!H95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="90">
+      <c r="A37" s="31">
+        <f>TODO!A96</f>
+        <v>94</v>
+      </c>
+      <c r="B37" s="36" t="str">
+        <f>TODO!B96</f>
+        <v>bug</v>
+      </c>
+      <c r="C37" t="str">
+        <f>TODO!C96</f>
+        <v>deleteBusiness</v>
+      </c>
+      <c r="D37" s="66">
+        <f>TODO!D96</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="50" t="str">
+        <f>TODO!E96</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/deleteBusiness/5058/2029
+{"Error":{"ErrorCode":"10"},"Result":"False","SuccessStatus":false}</v>
+      </c>
+      <c r="F37" s="41">
+        <f>TODO!F96</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="42" t="str">
+        <f>TODO!G96</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H37" s="69" t="str">
+        <f>TODO!H96</f>
+        <v>Confirmed!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="31">
+        <f>TODO!A98</f>
+        <v>96</v>
+      </c>
+      <c r="B38" s="31">
+        <f>TODO!B98</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="52" t="str">
+        <f>TODO!C98</f>
+        <v>5.20.2015</v>
+      </c>
+      <c r="D38" s="48">
+        <f>TODO!D98</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="46">
+        <f>TODO!E98</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="41">
+        <f>TODO!F98</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="41">
+        <f>TODO!G98</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="66">
+        <f>TODO!H98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="240">
+      <c r="A39" s="31">
+        <f>TODO!A99</f>
+        <v>97</v>
+      </c>
+      <c r="B39" s="36" t="str">
+        <f>TODO!B99</f>
+        <v>bug</v>
+      </c>
+      <c r="C39" t="str">
+        <f>TODO!C99</f>
+        <v>updatePost</v>
+      </c>
+      <c r="D39" s="45" t="str">
+        <f>TODO!D99</f>
+        <v>در متود ویرایش اطلاعات یک پست اگر تصویر
+پست (رشته) به صورت یک رشته تهی "" به سرور
+ارسال شود، فرض بر عدم تغییر تصویر فعلی پست در
+سرور است، در حالتی که وب سرویس مربوطه یک تصویر تهی برای آن پست ایجاد میکند و در دیتابیس قرار میدهد. 
+ویرایش اطلاعات پست با شناسه عددی ۳۱۵۸ بصورت گفته شده در بالا انجام شد
+سپس سرور یک تصویر تهی با شناسه عددی ۶۳۱۹
+را به آن اختصاص داد.</v>
+      </c>
+      <c r="E39" s="45" t="str">
+        <f>TODO!E99</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserPost/2029/3158
+{"Error":{"ErrorCode":null},"Result":"{\"UserId\":2029,\"BusinessId\":3034,\"PostId\":3158,\"UserName\":\"hamid1\",\"BusinessName\":null,\"Title\":\"hhggfg\",\"CreationDate\":\"433\",\"PostPictureId\":6319,\"BusinessProfilePictureId\":5410,\"Code\":\"\",\"Price\":\"\",\"Comments\":\"[{\\\"CommentId\\\":3066,\\\"User_Id\\\":2029,\\\"UserId\\\":null,\\\"UserName\\\":\\\"حميد 1\\\",\\\"Text\\\":\\\"تلنذب\\\",\\\"ProfilePictureId\\\":2022}]\",\"Description\":\"tozihaat\",\"IsLiked\":false,\"IsShared\":false,\"IsReported\":true,\"HashTagList\":\"\"}","SuccessStatus":true}</v>
+      </c>
+      <c r="F39" s="41">
+        <f>TODO!F99</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="42" t="str">
+        <f>TODO!G99</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H39" s="26" t="str">
+        <f>TODO!H99</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="120">
+      <c r="A40" s="31">
+        <f>TODO!A100</f>
+        <v>98</v>
+      </c>
+      <c r="B40" s="36" t="str">
+        <f>TODO!B100</f>
+        <v>bug</v>
+      </c>
+      <c r="C40" t="str">
+        <f>TODO!C100</f>
+        <v>GetUserFriendList</v>
+      </c>
+      <c r="D40" s="66" t="str">
+        <f>TODO!D100</f>
+        <v>It returns the own user as friend</v>
+      </c>
+      <c r="E40" s="45" t="str">
+        <f>TODO!E100</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserFriendList/2041
+"Result":"[{\"Id\":2041,\"UserId\":\"hamid10\",\"UserName\":\"hamid10\",\"UserProfilePictureId\":3258}
+,{\"Id\":2041,\"UserId\":\"hamid10\",\"UserName\":\"hamid10\",\"UserProfilePictureId\":3258}]</v>
+      </c>
+      <c r="F40" s="41">
+        <f>TODO!F100</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="42" t="str">
+        <f>TODO!G100</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H40" s="26" t="str">
+        <f>TODO!H100</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="255">
+      <c r="A41" s="31">
+        <f>TODO!A101</f>
+        <v>99</v>
+      </c>
+      <c r="B41" s="36" t="str">
+        <f>TODO!B101</f>
+        <v>bug</v>
+      </c>
+      <c r="C41" t="str">
+        <f>TODO!C101</f>
+        <v>UpdateBusinessProfileInfo</v>
+      </c>
+      <c r="D41" s="45" t="str">
+        <f>TODO!D101</f>
+        <v>{"SubCategoryId":"17","LocationLongitude":"51.3930864259601","Phone":"88359407",
+"Description":"همبرگر، هات داگ، سوسیس،#غذا","HashTagList":"غذ","CoverPicture":"",
+"WorkTimeClose":"17:40","WorkDays":"1,2,4","ProfilePicture":"","City":"تهران",
+"Name":"فست فوتی حمید","CategoryId":"16","State":"تهران","Email":"ggggggg@ggff.ir",
+"BusinessId":"3030","Address":"خيابان کريم خان،
+ خيابان نجات اللهي، کوجه شهيد هاشمي، پلاک 2، طبقه سوم، واحد 3","Mobile":"09359645502"
+,"LocationLatitude":"35.7226331860814","WorkTimeOpen":"08:21"}</v>
+      </c>
+      <c r="E41" s="66" t="str">
+        <f>TODO!E101</f>
+        <v>Error 10</v>
+      </c>
+      <c r="F41" s="41">
+        <f>TODO!F101</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="42" t="str">
+        <f>TODO!G101</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H41" s="26" t="str">
+        <f>TODO!H101</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="105">
+      <c r="A42" s="31">
+        <f>TODO!A102</f>
+        <v>100</v>
+      </c>
+      <c r="B42" s="36" t="str">
+        <f>TODO!B102</f>
+        <v>bug</v>
+      </c>
+      <c r="C42" t="str">
+        <f>TODO!C102</f>
+        <v>FollowBusiness</v>
+      </c>
+      <c r="D42" s="66" t="str">
+        <f>TODO!D102</f>
+        <v>when a user follows a business, a null post will be created for the business.</v>
+      </c>
+      <c r="E42" s="45" t="str">
+        <f>TODO!E102</f>
+        <v>وقتی که یک کاربر یک کسب و کار را دنبال میکند و url نمونه زیر اجرا میشود:
+http://185.55.226.223:8081/bsn/followBusiness/2029/3030
+علاوه بر اینکه عمل دنبال شدن آن کسب وکار توسط آن کاربر
+انجام میشود، یک پست تهی برای همان کسب و کار نیز در
+دیتابیس ایجاد میشود.</v>
+      </c>
+      <c r="F42" s="41">
+        <f>TODO!F102</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="42" t="str">
+        <f>TODO!G102</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H42" s="26" t="str">
+        <f>TODO!H102</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="31">
+        <f>TODO!A104</f>
+        <v>102</v>
+      </c>
+      <c r="B43" s="31">
+        <f>TODO!B104</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="52" t="str">
+        <f>TODO!C104</f>
+        <v>5.30.2015</v>
+      </c>
+      <c r="D43" s="66">
+        <f>TODO!D104</f>
+        <v>0</v>
+      </c>
+      <c r="E43" s="66">
+        <f>TODO!E104</f>
+        <v>0</v>
+      </c>
+      <c r="F43" s="41">
+        <f>TODO!F104</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="41">
+        <f>TODO!G104</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="66">
+        <f>TODO!H104</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="75">
+      <c r="A44" s="31">
+        <f>TODO!A105</f>
+        <v>103</v>
+      </c>
+      <c r="B44" s="36" t="str">
+        <f>TODO!B105</f>
+        <v>bug</v>
+      </c>
+      <c r="C44" t="str">
+        <f>TODO!C105</f>
+        <v>getBusinessReviews</v>
+      </c>
+      <c r="D44" s="66">
+        <f>TODO!D105</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="45" t="str">
+        <f>TODO!E105</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getBusinessReviews/3030/0/20
+Endpoint  not found</v>
+      </c>
+      <c r="F44" s="41">
+        <f>TODO!F105</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="42" t="str">
+        <f>TODO!G105</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H44" s="26" t="str">
+        <f>TODO!H105</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="120">
+      <c r="A45" s="31">
+        <f>TODO!A106</f>
+        <v>104</v>
+      </c>
+      <c r="B45" s="36" t="str">
+        <f>TODO!B106</f>
+        <v>bug</v>
+      </c>
+      <c r="C45" t="str">
+        <f>TODO!C106</f>
+        <v>GetUserHomeInfo</v>
+      </c>
+      <c r="D45" s="66" t="str">
+        <f>TODO!D106</f>
+        <v>faulty data</v>
+      </c>
+      <c r="E45" s="45" t="str">
+        <f>TODO!E106</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserHomeInfo/2036/2029 
+returns faulty data:
+{"Error":{"ErrorCode":"Sequence contains more than one element"},"Result":"","SuccessStatus":false}</v>
+      </c>
+      <c r="F45" s="41">
+        <f>TODO!F106</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="42" t="str">
+        <f>TODO!G106</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H45" s="26" t="str">
+        <f>TODO!H106</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="31">
+        <f>TODO!A108</f>
+        <v>106</v>
+      </c>
+      <c r="B46" s="31">
+        <f>TODO!B108</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="52" t="str">
+        <f>TODO!C108</f>
+        <v>5.31.2015</v>
+      </c>
+      <c r="D46" s="66">
+        <f>TODO!D108</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="66">
+        <f>TODO!E108</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="41">
+        <f>TODO!F108</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="41">
+        <f>TODO!G108</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="66">
+        <f>TODO!H108</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="90">
+      <c r="A47" s="31">
+        <f>TODO!A110</f>
+        <v>108</v>
+      </c>
+      <c r="B47" s="36" t="str">
+        <f>TODO!B110</f>
+        <v>bug</v>
+      </c>
+      <c r="C47" t="str">
+        <f>TODO!C110</f>
+        <v>deleteBusiness</v>
+      </c>
+      <c r="D47" s="60" t="str">
+        <f>TODO!D110</f>
+        <v>وب سرویس پاک کردن یک کسب و کار عمل نمیکند.
+کسب و کار مربوطه از دیتابیس پاک نمیشود.</v>
+      </c>
+      <c r="E47" s="11" t="str">
+        <f>TODO!E110</f>
+        <v>sample url:
+http://185.55.226.223:8081/bsn/deleteBusiness/5055/2029
+{"Error":{"ErrorCode":null},"Result":"False","SuccessStatus":true}</v>
+      </c>
+      <c r="F47" s="66">
+        <f>TODO!F110</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="42" t="str">
+        <f>TODO!G110</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H47" s="26" t="str">
+        <f>TODO!H110</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="31">
+        <f>TODO!A112</f>
+        <v>0</v>
+      </c>
+      <c r="B48" s="52" t="str">
+        <f>TODO!B112</f>
+        <v>6.1.2015</v>
+      </c>
+      <c r="C48" s="52" t="str">
+        <f>TODO!C112</f>
+        <v>6.1.2015</v>
+      </c>
+      <c r="D48" s="52" t="str">
+        <f>TODO!D112</f>
+        <v>6.1.2015</v>
+      </c>
+      <c r="E48" s="52" t="str">
+        <f>TODO!E112</f>
+        <v>6.1.2015</v>
+      </c>
+      <c r="F48" s="52" t="str">
+        <f>TODO!F112</f>
+        <v>6.1.2015</v>
+      </c>
+      <c r="G48" s="52" t="str">
+        <f>TODO!G112</f>
+        <v>6.1.2015</v>
+      </c>
+      <c r="H48" s="52" t="str">
+        <f>TODO!H112</f>
+        <v>6.1.2015</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="31">
+        <f>TODO!A113</f>
+        <v>109</v>
+      </c>
+      <c r="B49" s="36" t="str">
+        <f>TODO!B113</f>
+        <v>bug</v>
+      </c>
+      <c r="C49" s="66" t="str">
+        <f>TODO!C113</f>
+        <v>RegisterUser(method name: registerUser)</v>
+      </c>
+      <c r="D49" s="66">
+        <f>TODO!D113</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="66" t="str">
+        <f>TODO!E113</f>
+        <v>{"Error":{"ErrorCode":"Incorrect number of arguments supplied for call to method 'Boolean Equals(System.String, System.String, System.StringComparison)'"},"Result":"","SuccessStatus":false}</v>
+      </c>
+      <c r="F49" s="66">
+        <f>TODO!F113</f>
+        <v>0</v>
+      </c>
+      <c r="G49" s="42" t="str">
+        <f>TODO!G113</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H49" s="26" t="str">
+        <f>TODO!H113</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="195">
+      <c r="A50" s="31">
+        <f>TODO!A114</f>
+        <v>110</v>
+      </c>
+      <c r="B50" s="36" t="str">
+        <f>TODO!B114</f>
+        <v>bug</v>
+      </c>
+      <c r="C50" s="45" t="str">
+        <f>TODO!C114</f>
+        <v>Android Class: GetPost
+server method: getUserPost</v>
+      </c>
+      <c r="D50" s="66" t="str">
+        <f>TODO!D114</f>
+        <v>مقادیر بعضی فیلدها در پاسخ سرور به صورت نال است.</v>
+      </c>
+      <c r="E50" s="45" t="str">
+        <f>TODO!E114</f>
+        <v>sample URL:
+http://185.55.226.223:8081/bsn/getUserPost/2029/4075
+Result:
+{"Error":{"ErrorCode":null},"Result":"{\"UserId\":2029,\"BusinessId\":3030,\"PostId\":4075,\"UserName\":\"hamid1\",\"BusinessName\":null,\"Title\":null,\"CreationDate\":\"20\",\"PostPictureId\":0,\"BusinessProfilePictureId\":5410,\"Code\":null,\"Price\":null,\"Comments\":\"[]\",\"Description\":null,\"IsLiked\":false,\"IsShared\":false,\"IsReported\":false,\"HashTagList\":null}","SuccessStatus":true}</v>
+      </c>
+      <c r="F50" s="66">
+        <f>TODO!F114</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="42" t="str">
+        <f>TODO!G114</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H50" s="26" t="str">
+        <f>TODO!H114</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="90">
+      <c r="A51" s="31">
+        <f>TODO!A115</f>
+        <v>111</v>
+      </c>
+      <c r="B51" s="36" t="str">
+        <f>TODO!B115</f>
+        <v>bug</v>
+      </c>
+      <c r="C51" s="66" t="str">
+        <f>TODO!C115</f>
+        <v>registerBusiness</v>
+      </c>
+      <c r="D51" s="45" t="str">
+        <f>TODO!D115</f>
+        <v>یک کد خطا برمیگرداند که گمان میکنم مربوط به تابع
+بررسی کننده یکتایی شناسه حرفی کسب و کار باشد</v>
+      </c>
+      <c r="E51" s="45" t="str">
+        <f>TODO!E115</f>
+        <v>{"Error":{"ErrorCode":"Incorrect number of arguments
+supplied for call to method 'Boolean Equals(System.String
+, System.String, System.StringComparison)'"},"
+Result":"","SuccessStatus":false}</v>
+      </c>
+      <c r="F51" s="66">
+        <f>TODO!F115</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="42" t="str">
+        <f>TODO!G115</f>
+        <v>Reviewed!</v>
+      </c>
+      <c r="H51" s="26" t="str">
+        <f>TODO!H115</f>
+        <v>Waiting For Change!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E110"/>
   <sheetViews>
@@ -5420,7 +7518,7 @@
       <c r="A78" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B78" s="67" t="s">
+      <c r="B78" s="68" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5428,19 +7526,19 @@
       <c r="A79" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="67"/>
+      <c r="B79" s="68"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="67"/>
+      <c r="B80" s="68"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="67"/>
+      <c r="B81" s="68"/>
     </row>
     <row r="82" spans="1:3" ht="300">
       <c r="A82" s="19" t="s">

</xml_diff>

<commit_message>
Fixed Bug: vaghti karbar be safeye dustane khodash miravad, agar darkhaste dusti nadashte bashad dokmeye darkhasthaye dusti mahv mishavad, hal agar darkhaste dusti jadid barayash biayad, dokme mazkur ba khoruj az barname va vorude dobare visible mishavad
webservices_bugs.xlsx updated with new Bugs!
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
     <sheet name="WebServices With Bug" sheetId="5" r:id="rId2"/>
-    <sheet name="Trash" sheetId="1" r:id="rId3"/>
+    <sheet name="Webservices To Change" sheetId="6" r:id="rId3"/>
+    <sheet name="New Webservice Needs" sheetId="7" r:id="rId4"/>
+    <sheet name="Trash" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="257">
   <si>
     <t>UnFollowBusiness</t>
   </si>
@@ -1987,6 +1989,21 @@
       </rPr>
       <t>,\"BusinessProfilePictureId\":5410,\"Code\":\"\",\"Price\":\"\",\"Comments\":\"[{\\\"CommentId\\\":3066,\\\"User_Id\\\":2029,\\\"UserId\\\":null,\\\"UserName\\\":\\\"حميد 1\\\",\\\"Text\\\":\\\"تلنذب\\\",\\\"ProfilePictureId\\\":2022}]\",\"Description\":\"tozihaat\",\"IsLiked\":false,\"IsShared\":false,\"IsReported\":true,\"HashTagList\":\"\"}","SuccessStatus":true}</t>
     </r>
+  </si>
+  <si>
+    <t>sample url:
+http://185.55.226.223:8081/bsn/getUserHomeInfo/2029/2037
+result:
+{"Error":{"ErrorCode":"Sequence contains more than one element"},"Result":"","SuccessStatus":false}</t>
+  </si>
+  <si>
+    <t>کاربر hamid6 وقتی از صفحه نتایج سرچ با
+فراخوانی متود GetUserHomeInfo میخواهد
+به صفحه پروفایل کاربر Hamid1 هدایت شود
+با خطا مواجه میشود</t>
+  </si>
+  <si>
+    <t>6.7.2015</t>
   </si>
 </sst>
 </file>
@@ -2279,7 +2296,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2476,9 +2493,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2494,6 +2508,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2786,13 +2806,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I116"/>
+  <dimension ref="A2:I118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3055,7 +3075,7 @@
       <c r="G13" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H13" s="69" t="s">
+      <c r="H13" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3079,7 +3099,7 @@
       <c r="G14" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H14" s="69" t="s">
+      <c r="H14" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3296,7 +3316,7 @@
       <c r="G26" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H26" s="69" t="s">
+      <c r="H26" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3371,7 +3391,7 @@
       <c r="G30" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H30" s="69" t="s">
+      <c r="H30" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3438,7 +3458,7 @@
       <c r="G34" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H34" s="71" t="s">
+      <c r="H34" s="70" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3480,7 +3500,7 @@
       <c r="G36" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H36" s="69" t="s">
+      <c r="H36" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3559,7 +3579,7 @@
       <c r="G41" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H41" s="72" t="s">
+      <c r="H41" s="71" t="s">
         <v>248</v>
       </c>
     </row>
@@ -3681,7 +3701,7 @@
       <c r="G47" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H47" s="71" t="s">
+      <c r="H47" s="70" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3702,7 +3722,7 @@
       <c r="G48" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H48" s="69" t="s">
+      <c r="H48" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3741,7 +3761,7 @@
       <c r="G51" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H51" s="69" t="s">
+      <c r="H51" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3762,7 +3782,7 @@
       <c r="G52" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H52" s="70" t="s">
+      <c r="H52" s="69" t="s">
         <v>199</v>
       </c>
     </row>
@@ -3995,7 +4015,7 @@
       <c r="G65" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H65" s="69" t="s">
+      <c r="H65" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4128,7 +4148,7 @@
       <c r="G73" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H73" s="73" t="s">
+      <c r="H73" s="72" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4189,7 +4209,7 @@
       <c r="G76" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H76" s="69" t="s">
+      <c r="H76" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4210,7 +4230,7 @@
       <c r="G77" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H77" s="69" t="s">
+      <c r="H77" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4272,7 +4292,7 @@
       <c r="C80" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="67" t="s">
+      <c r="D80" s="74" t="s">
         <v>135</v>
       </c>
       <c r="F80" s="41"/>
@@ -4288,7 +4308,7 @@
       <c r="C81" t="s">
         <v>29</v>
       </c>
-      <c r="D81" s="67"/>
+      <c r="D81" s="74"/>
       <c r="F81" s="41"/>
       <c r="G81" s="41"/>
     </row>
@@ -4302,7 +4322,7 @@
       <c r="C82" t="s">
         <v>63</v>
       </c>
-      <c r="D82" s="67"/>
+      <c r="D82" s="74"/>
       <c r="F82" s="41"/>
       <c r="G82" s="41"/>
     </row>
@@ -4316,7 +4336,7 @@
       <c r="C83" t="s">
         <v>16</v>
       </c>
-      <c r="D83" s="67"/>
+      <c r="D83" s="74"/>
       <c r="F83" s="41"/>
       <c r="G83" s="41"/>
     </row>
@@ -4337,7 +4357,7 @@
       <c r="G84" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H84" s="69" t="s">
+      <c r="H84" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4358,7 +4378,7 @@
       <c r="G85" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H85" s="69" t="s">
+      <c r="H85" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4382,7 +4402,7 @@
       <c r="G86" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H86" s="69" t="s">
+      <c r="H86" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4405,19 +4425,19 @@
       <c r="G88" s="41"/>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="74">
+      <c r="A89" s="73">
         <v>87</v>
       </c>
-      <c r="B89" s="74" t="s">
+      <c r="B89" s="73" t="s">
         <v>251</v>
       </c>
-      <c r="C89" s="74" t="s">
+      <c r="C89" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="D89" s="74" t="s">
+      <c r="D89" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="E89" s="74" t="s">
+      <c r="E89" s="73" t="s">
         <v>78</v>
       </c>
       <c r="F89" s="41"/>
@@ -4459,7 +4479,7 @@
       <c r="G92" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H92" s="69" t="s">
+      <c r="H92" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4514,7 +4534,7 @@
       <c r="G96" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H96" s="69" t="s">
+      <c r="H96" s="68" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4834,31 +4854,77 @@
         <v>226</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="90">
-      <c r="A115" s="31">
+    <row r="115" spans="1:8">
+      <c r="B115"/>
+      <c r="C115" s="45"/>
+      <c r="D115" s="67"/>
+      <c r="E115" s="45"/>
+      <c r="F115" s="67"/>
+      <c r="G115"/>
+      <c r="H115"/>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="B116" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="C116" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="D116" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="E116" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="F116" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="G116" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="H116" s="52" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="90">
+      <c r="A117" s="31">
         <v>111</v>
       </c>
-      <c r="B115" s="36" t="s">
+      <c r="B117" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C115" s="39" t="s">
+      <c r="C117" s="39" t="s">
         <v>245</v>
       </c>
-      <c r="D115" s="45" t="s">
+      <c r="D117" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="E115" s="45" t="s">
+      <c r="E117" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="G115" s="42" t="s">
+      <c r="G117" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="H115" s="26" t="s">
+      <c r="H117" s="26" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
-      <c r="C116" s="64"/>
+    <row r="118" spans="1:8" ht="105">
+      <c r="A118" s="31">
+        <v>112</v>
+      </c>
+      <c r="B118" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C118" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D118" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="E118" s="45" t="s">
+        <v>254</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4873,11 +4939,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4950,7 +5016,7 @@
         <f>TODO!G13</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H3" s="69" t="str">
+      <c r="H3" s="68" t="str">
         <f>TODO!H13</f>
         <v>Confirmed!</v>
       </c>
@@ -4987,7 +5053,7 @@
         <f>TODO!G14</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H4" s="69" t="str">
+      <c r="H4" s="68" t="str">
         <f>TODO!H14</f>
         <v>Confirmed!</v>
       </c>
@@ -5169,7 +5235,7 @@
         <f>TODO!G26</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H9" s="69" t="str">
+      <c r="H9" s="68" t="str">
         <f>TODO!H26</f>
         <v>Confirmed!</v>
       </c>
@@ -5203,7 +5269,7 @@
         <f>TODO!G30</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H10" s="69" t="str">
+      <c r="H10" s="68" t="str">
         <f>TODO!H30</f>
         <v>Confirmed!</v>
       </c>
@@ -5318,7 +5384,7 @@
         <f>TODO!G34</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H13" s="71" t="str">
+      <c r="H13" s="70" t="str">
         <f>TODO!H34</f>
         <v>Confirmed!
 تغییر اعمال شده است اما
@@ -5361,7 +5427,7 @@
         <f>TODO!G36</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H14" s="69" t="str">
+      <c r="H14" s="68" t="str">
         <f>TODO!H36</f>
         <v>Confirmed!</v>
       </c>
@@ -5430,7 +5496,7 @@
         <f>TODO!G41</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H16" s="72" t="str">
+      <c r="H16" s="71" t="str">
         <f>TODO!H41</f>
         <v>NOT Confirmed!
 با توجه به اینکه ثبت کسب
@@ -5472,7 +5538,7 @@
         <f>TODO!G47</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H17" s="71" t="str">
+      <c r="H17" s="70" t="str">
         <f>TODO!H47</f>
         <v>NOT Confirmed!
 با توجه به وجود باگ شماره
@@ -5516,7 +5582,7 @@
         <f>TODO!G48</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H18" s="69" t="str">
+      <c r="H18" s="68" t="str">
         <f>TODO!H48</f>
         <v>Confirmed!</v>
       </c>
@@ -5586,7 +5652,7 @@
         <f>TODO!G51</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H20" s="69" t="str">
+      <c r="H20" s="68" t="str">
         <f>TODO!H51</f>
         <v>Confirmed!</v>
       </c>
@@ -5620,7 +5686,7 @@
         <f>TODO!G52</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H21" s="70" t="str">
+      <c r="H21" s="69" t="str">
         <f>TODO!H52</f>
         <v>NOT Confirmed!</v>
       </c>
@@ -5690,7 +5756,7 @@
         <f>TODO!G65</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H23" s="69" t="str">
+      <c r="H23" s="68" t="str">
         <f>TODO!H65</f>
         <v>Confirmed!</v>
       </c>
@@ -5762,7 +5828,7 @@
         <f>TODO!G73</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H25" s="73" t="str">
+      <c r="H25" s="72" t="str">
         <f>TODO!H73</f>
         <v>Confirmed!
 یکی از باگها حل شده
@@ -5840,7 +5906,7 @@
         <f>TODO!G76</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H27" s="69" t="str">
+      <c r="H27" s="68" t="str">
         <f>TODO!H76</f>
         <v>Confirmed!</v>
       </c>
@@ -5895,7 +5961,7 @@
         <f>TODO!G77</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H28" s="69" t="str">
+      <c r="H28" s="68" t="str">
         <f>TODO!H77</f>
         <v>Confirmed!</v>
       </c>
@@ -6009,7 +6075,7 @@
         <f>TODO!G84</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H31" s="69" t="str">
+      <c r="H31" s="68" t="str">
         <f>TODO!H84</f>
         <v>Confirmed!</v>
       </c>
@@ -6046,7 +6112,7 @@
         <f>TODO!G85</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H32" s="69" t="str">
+      <c r="H32" s="68" t="str">
         <f>TODO!H85</f>
         <v>Confirmed!</v>
       </c>
@@ -6080,7 +6146,7 @@
         <f>TODO!G86</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H33" s="69" t="str">
+      <c r="H33" s="68" t="str">
         <f>TODO!H86</f>
         <v>Confirmed!</v>
       </c>
@@ -6151,7 +6217,7 @@
         <f>TODO!G92</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H35" s="69" t="str">
+      <c r="H35" s="68" t="str">
         <f>TODO!H92</f>
         <v>Confirmed!</v>
       </c>
@@ -6221,7 +6287,7 @@
         <f>TODO!G96</f>
         <v>Reviewed!</v>
       </c>
-      <c r="H37" s="69" t="str">
+      <c r="H37" s="68" t="str">
         <f>TODO!H96</f>
         <v>Confirmed!</v>
       </c>
@@ -6703,39 +6769,39 @@
     </row>
     <row r="51" spans="1:8" ht="90">
       <c r="A51" s="31">
-        <f>TODO!A115</f>
+        <f>TODO!A117</f>
         <v>111</v>
       </c>
       <c r="B51" s="36" t="str">
-        <f>TODO!B115</f>
+        <f>TODO!B117</f>
         <v>bug</v>
       </c>
       <c r="C51" s="66" t="str">
-        <f>TODO!C115</f>
+        <f>TODO!C117</f>
         <v>registerBusiness</v>
       </c>
       <c r="D51" s="45" t="str">
-        <f>TODO!D115</f>
+        <f>TODO!D117</f>
         <v>یک کد خطا برمیگرداند که گمان میکنم مربوط به تابع
 بررسی کننده یکتایی شناسه حرفی کسب و کار باشد</v>
       </c>
       <c r="E51" s="45" t="str">
-        <f>TODO!E115</f>
+        <f>TODO!E117</f>
         <v>{"Error":{"ErrorCode":"Incorrect number of arguments
 supplied for call to method 'Boolean Equals(System.String
 , System.String, System.StringComparison)'"},"
 Result":"","SuccessStatus":false}</v>
       </c>
       <c r="F51" s="66">
-        <f>TODO!F115</f>
+        <f>TODO!F117</f>
         <v>0</v>
       </c>
       <c r="G51" s="42" t="str">
-        <f>TODO!G115</f>
+        <f>TODO!G117</f>
         <v>Reviewed!</v>
       </c>
       <c r="H51" s="26" t="str">
-        <f>TODO!H115</f>
+        <f>TODO!H117</f>
         <v>Waiting For Change!</v>
       </c>
     </row>
@@ -6746,6 +6812,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E110"/>
   <sheetViews>
@@ -7518,7 +7608,7 @@
       <c r="A78" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B78" s="68" t="s">
+      <c r="B78" s="75" t="s">
         <v>135</v>
       </c>
     </row>
@@ -7526,19 +7616,19 @@
       <c r="A79" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="68"/>
+      <c r="B79" s="75"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="68"/>
+      <c r="B80" s="75"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="68"/>
+      <c r="B81" s="75"/>
     </row>
     <row r="82" spans="1:3" ht="300">
       <c r="A82" s="19" t="s">

</xml_diff>

<commit_message>
fixed bugs: 2 buge digar dar namayeshe dokmeye darkhasthaye dusti dar safeye dustane karbar bartaraf shod.
webservices_bugs.xlsx updated!
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="259">
   <si>
     <t>UnFollowBusiness</t>
   </si>
@@ -2004,6 +2004,19 @@
   </si>
   <si>
     <t>6.7.2015</t>
+  </si>
+  <si>
+    <t>وقتی درخواست دوستی درخواست کننده(hamid15
+با شناسه عددی 2046) توسط درخواست شونده
+(hamid6 با شناسه عددی 2037) تایید میشود،
+hamid15 میتواند hamid6 را در لیست دوستانش
+ببیند اما hamid6 نمیتواند hamid15 را ببیند</t>
+  </si>
+  <si>
+    <t>sample URL(Hamid15 Friendlist):
+http://185.55.226.223:8081/bsn/getUserFriendList/2046
+sample URL(Hamid6 Friendlist):
+http://185.55.226.223:8081/bsn/getUserFriendList/2037</t>
   </si>
 </sst>
 </file>
@@ -2296,7 +2309,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2507,6 +2520,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="4" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2806,13 +2822,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I118"/>
+  <dimension ref="A2:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D115" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D117" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F114" sqref="F114"/>
+      <selection pane="bottomRight" activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4292,7 +4308,7 @@
       <c r="C80" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="74" t="s">
+      <c r="D80" s="75" t="s">
         <v>135</v>
       </c>
       <c r="F80" s="41"/>
@@ -4308,7 +4324,7 @@
       <c r="C81" t="s">
         <v>29</v>
       </c>
-      <c r="D81" s="74"/>
+      <c r="D81" s="75"/>
       <c r="F81" s="41"/>
       <c r="G81" s="41"/>
     </row>
@@ -4322,7 +4338,7 @@
       <c r="C82" t="s">
         <v>63</v>
       </c>
-      <c r="D82" s="74"/>
+      <c r="D82" s="75"/>
       <c r="F82" s="41"/>
       <c r="G82" s="41"/>
     </row>
@@ -4336,7 +4352,7 @@
       <c r="C83" t="s">
         <v>16</v>
       </c>
-      <c r="D83" s="74"/>
+      <c r="D83" s="75"/>
       <c r="F83" s="41"/>
       <c r="G83" s="41"/>
     </row>
@@ -4924,6 +4940,23 @@
       </c>
       <c r="E118" s="45" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="105">
+      <c r="A119" s="31">
+        <v>113</v>
+      </c>
+      <c r="B119" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C119" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D119" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="E119" s="45" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -4937,13 +4970,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H51"/>
+  <dimension ref="A2:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomRight" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6803,6 +6836,87 @@
       <c r="H51" s="26" t="str">
         <f>TODO!H117</f>
         <v>Waiting For Change!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="105">
+      <c r="A52" s="31">
+        <f>TODO!A118</f>
+        <v>112</v>
+      </c>
+      <c r="B52" s="36" t="str">
+        <f>TODO!B118</f>
+        <v>bug</v>
+      </c>
+      <c r="C52" s="74" t="str">
+        <f>TODO!C118</f>
+        <v>GetUserHomeInfo</v>
+      </c>
+      <c r="D52" s="45" t="str">
+        <f>TODO!D118</f>
+        <v>کاربر hamid6 وقتی از صفحه نتایج سرچ با
+فراخوانی متود GetUserHomeInfo میخواهد
+به صفحه پروفایل کاربر Hamid1 هدایت شود
+با خطا مواجه میشود</v>
+      </c>
+      <c r="E52" s="45" t="str">
+        <f>TODO!E118</f>
+        <v>sample url:
+http://185.55.226.223:8081/bsn/getUserHomeInfo/2029/2037
+result:
+{"Error":{"ErrorCode":"Sequence contains more than one element"},"Result":"","SuccessStatus":false}</v>
+      </c>
+      <c r="F52" s="74">
+        <f>TODO!F118</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="74">
+        <f>TODO!G118</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="74">
+        <f>TODO!H118</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="105">
+      <c r="A53" s="31">
+        <f>TODO!A119</f>
+        <v>113</v>
+      </c>
+      <c r="B53" s="36" t="str">
+        <f>TODO!B119</f>
+        <v>bug</v>
+      </c>
+      <c r="C53" s="74" t="str">
+        <f>TODO!C119</f>
+        <v>getUserFriendList</v>
+      </c>
+      <c r="D53" s="45" t="str">
+        <f>TODO!D119</f>
+        <v>وقتی درخواست دوستی درخواست کننده(hamid15
+با شناسه عددی 2046) توسط درخواست شونده
+(hamid6 با شناسه عددی 2037) تایید میشود،
+hamid15 میتواند hamid6 را در لیست دوستانش
+ببیند اما hamid6 نمیتواند hamid15 را ببیند</v>
+      </c>
+      <c r="E53" s="45" t="str">
+        <f>TODO!E119</f>
+        <v>sample URL(Hamid15 Friendlist):
+http://185.55.226.223:8081/bsn/getUserFriendList/2046
+sample URL(Hamid6 Friendlist):
+http://185.55.226.223:8081/bsn/getUserFriendList/2037</v>
+      </c>
+      <c r="F53" s="74">
+        <f>TODO!F119</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="74">
+        <f>TODO!G119</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="74">
+        <f>TODO!H119</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7608,7 +7722,7 @@
       <c r="A78" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B78" s="75" t="s">
+      <c r="B78" s="76" t="s">
         <v>135</v>
       </c>
     </row>
@@ -7616,19 +7730,19 @@
       <c r="A79" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="75"/>
+      <c r="B79" s="76"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="75"/>
+      <c r="B80" s="76"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="75"/>
+      <c r="B81" s="76"/>
     </row>
     <row r="82" spans="1:3" ht="300">
       <c r="A82" s="19" t="s">

</xml_diff>

<commit_message>
newly added: 2 LEVEL SignUp
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="260">
   <si>
     <t>UnFollowBusiness</t>
   </si>
@@ -2017,6 +2017,10 @@
 http://185.55.226.223:8081/bsn/getUserFriendList/2046
 sample URL(Hamid6 Friendlist):
 http://185.55.226.223:8081/bsn/getUserFriendList/2037</t>
+  </si>
+  <si>
+    <t>لطفا شناسه عددی کامنت ثبت شده را با فرمت JSON 
+با کلید commentId_int در پاسخ سرور قرار بدید</t>
   </si>
 </sst>
 </file>
@@ -2824,11 +2828,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D117" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G118" sqref="G118:H119"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3354,7 +3358,7 @@
       </c>
       <c r="G27" s="41"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" ht="30">
       <c r="A28" s="31">
         <v>26</v>
       </c>
@@ -3367,10 +3371,16 @@
       <c r="D28" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="G28" s="41"/>
+      <c r="E28" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="F28" s="41"/>
+      <c r="G28" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H28" s="44" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="31">
@@ -4984,8 +4994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D90" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="E52" sqref="E52"/>

</xml_diff>

<commit_message>
sabte name 3 sathi kamel shod.
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Android\Dev\4Soo2\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AndroidDev\Charsoo\4Soo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2976,10 +2976,10 @@
   <dimension ref="A2:H122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D119" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A122" sqref="A122"/>
+      <selection pane="bottomRight" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
some bugs fixed. date management added.
</commit_message>
<xml_diff>
--- a/docs/webservices_bugs.xlsx
+++ b/docs/webservices_bugs.xlsx
@@ -2976,10 +2976,10 @@
   <dimension ref="A2:H122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D120" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F66" sqref="F66"/>
+      <selection pane="bottomRight" activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>